<commit_message>
Fixed error in SampleInfo.
The header info for the run starting 141021 was incorrect.
I've also added sheets that are named identically to the subfolders in
the LS6500. These sheets also contain the measurement ordering.
</commit_message>
<xml_diff>
--- a/SampleInfo.xlsx
+++ b/SampleInfo.xlsx
@@ -14,13 +14,18 @@
     <sheet name="LS Measurement arrangement" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Storage Matrix" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Notes" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Pre-irrad_1_141014" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Gamma_Pre-irradiation141017" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Gamma_1Gy_141020" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Gamma_All_141021" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Gamma_All_141022" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="329">
   <si>
     <t>Irradiation #</t>
   </si>
@@ -749,6 +754,15 @@
   </si>
   <si>
     <t>Gamma Post-irradiation measurements 141020 (actual)</t>
+  </si>
+  <si>
+    <t>Gamma Post-irradiation measurements 141021 (actual)</t>
+  </si>
+  <si>
+    <t>Gamma Post-irradiation Measurements 141022 (actual)</t>
+  </si>
+  <si>
+    <t>HDPE_0_1</t>
   </si>
   <si>
     <t>Post-irradiation measurements (planned)</t>
@@ -1263,7 +1277,6 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C6"/>
@@ -1327,10 +1340,764 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="9" t="str">
+        <f aca="false">'LS Measurement arrangement'!B36</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C36</f>
+        <v>0050_0_1</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D36</f>
+        <v>0050_0_2</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E36</f>
+        <v>0052_0_1</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F36</f>
+        <v>0052_0_2</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G36</f>
+        <v>0050_100_1</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H36</f>
+        <v>0050_100_2</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I36</f>
+        <v>0052_100_1</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J36</f>
+        <v>0052_100_2</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K36</f>
+        <v>0050_400_1</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L36</f>
+        <v>0050_400_2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B37</f>
+        <v>0052_400_1</v>
+      </c>
+      <c r="C3" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!C37</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D37</f>
+        <v>0052_400_2</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E37</f>
+        <v>0100_0_1</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F37</f>
+        <v>0100_0_2</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G37</f>
+        <v>0102_0_1</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H37</f>
+        <v>0102_0_2</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I37</f>
+        <v>0100_1_1</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J37</f>
+        <v>0100_1_2</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K37</f>
+        <v>0102_1_1</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L37</f>
+        <v>0102_1_2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B38</f>
+        <v>0100_10_1</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C38</f>
+        <v>0100_10_2</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!D38</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E38</f>
+        <v>0102_10_1</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F38</f>
+        <v>0102_10_2</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G38</f>
+        <v>0100_100_1</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H38</f>
+        <v>0100_100_2</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I38</f>
+        <v>0102_100_1</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J38</f>
+        <v>0102_100_2</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K38</f>
+        <v>0100_400_1</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L38</f>
+        <v>0100_400_2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B39</f>
+        <v>0102_400_1</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C39</f>
+        <v>0102_400_2</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D39</f>
+        <v>0100_1000_1</v>
+      </c>
+      <c r="E5" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!E39</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F39</f>
+        <v>0100_1000_2</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G39</f>
+        <v>0102_1000_1</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H39</f>
+        <v>0102_1000_2</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I39</f>
+        <v>GLASS_0_1</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J39</f>
+        <v>GLASS_0_2</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K39</f>
+        <v>PP_0_1</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L39</f>
+        <v>PP_0_2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B40</f>
+        <v>GLASS_100_1</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C40</f>
+        <v>GLASS_100_2</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D40</f>
+        <v>PP_100_1</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E40</f>
+        <v>PP_100_2</v>
+      </c>
+      <c r="F6" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!F40</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G40</f>
+        <v>GLASS_400_1</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H40</f>
+        <v>GLASS_400_2</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I40</f>
+        <v>PP_400_1</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J40</f>
+        <v>PP_400_2</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K40</f>
+        <v>GLASS_1000_1</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L40</f>
+        <v>GLASS_1000_2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B41</f>
+        <v>PP_1000_1</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C41</f>
+        <v>PP_1000_2</v>
+      </c>
+      <c r="G7" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!G41</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B42</f>
+        <v>LS Vit. C</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C42</f>
+        <v>15% WbLS Vit. C</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D42</f>
+        <v>10% WbLS Vit. C</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E42</f>
+        <v>5% WbLS Vit. C</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F42</f>
+        <v>LS 10/20/14</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G42</f>
+        <v>WbLS-15 10/20/14</v>
+      </c>
+      <c r="H8" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!H42</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I42</f>
+        <v>WbLS-10 10/20/14</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J42</f>
+        <v>WbLS-5 10/20/14</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="9" t="str">
+        <f aca="false">'LS Measurement arrangement'!B47</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!C47</f>
+        <v>0050_0_1</v>
+      </c>
+      <c r="D2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!D47</f>
+        <v>0050_0_2</v>
+      </c>
+      <c r="E2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!E47</f>
+        <v>0052_0_1</v>
+      </c>
+      <c r="F2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!F47</f>
+        <v>0052_0_2</v>
+      </c>
+      <c r="G2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!G47</f>
+        <v>0050_100_1</v>
+      </c>
+      <c r="H2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!H47</f>
+        <v>0050_100_2</v>
+      </c>
+      <c r="I2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!I47</f>
+        <v>0052_100_1</v>
+      </c>
+      <c r="J2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!J47</f>
+        <v>0052_100_2</v>
+      </c>
+      <c r="K2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!K47</f>
+        <v>0050_400_1</v>
+      </c>
+      <c r="L2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!L47</f>
+        <v>0050_400_2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B48</f>
+        <v>0052_400_1</v>
+      </c>
+      <c r="C3" s="9" t="str">
+        <f aca="false">'LS Measurement arrangement'!C48</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="D3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!D48</f>
+        <v>0052_400_2</v>
+      </c>
+      <c r="E3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!E48</f>
+        <v>0100_0_1</v>
+      </c>
+      <c r="F3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!F48</f>
+        <v>0100_0_2</v>
+      </c>
+      <c r="G3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!G48</f>
+        <v>0102_0_1</v>
+      </c>
+      <c r="H3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!H48</f>
+        <v>0102_0_2</v>
+      </c>
+      <c r="I3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!I48</f>
+        <v>0100_1_1</v>
+      </c>
+      <c r="J3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!J48</f>
+        <v>0100_1_2</v>
+      </c>
+      <c r="K3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!K48</f>
+        <v>0102_1_1</v>
+      </c>
+      <c r="L3" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!L48</f>
+        <v>0102_1_2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B49</f>
+        <v>0100_10_1</v>
+      </c>
+      <c r="C4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!C49</f>
+        <v>0100_10_2</v>
+      </c>
+      <c r="D4" s="9" t="str">
+        <f aca="false">'LS Measurement arrangement'!D49</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!E49</f>
+        <v>0102_10_1</v>
+      </c>
+      <c r="F4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!F49</f>
+        <v>0102_10_2</v>
+      </c>
+      <c r="G4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!G49</f>
+        <v>0100_100_1</v>
+      </c>
+      <c r="H4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!H49</f>
+        <v>0100_100_2</v>
+      </c>
+      <c r="I4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!I49</f>
+        <v>0102_100_1</v>
+      </c>
+      <c r="J4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!J49</f>
+        <v>0102_100_2</v>
+      </c>
+      <c r="K4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!K49</f>
+        <v>0100_400_1</v>
+      </c>
+      <c r="L4" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!L49</f>
+        <v>0100_400_2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B50</f>
+        <v>0102_400_1</v>
+      </c>
+      <c r="C5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!C50</f>
+        <v>0102_400_2</v>
+      </c>
+      <c r="D5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!D50</f>
+        <v>0100_1000_1</v>
+      </c>
+      <c r="E5" s="9" t="str">
+        <f aca="false">'LS Measurement arrangement'!E50</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!F50</f>
+        <v>0100_1000_2</v>
+      </c>
+      <c r="G5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!G50</f>
+        <v>0102_1000_1</v>
+      </c>
+      <c r="H5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!H50</f>
+        <v>0102_1000_2</v>
+      </c>
+      <c r="I5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!I50</f>
+        <v>GLASS_0_1</v>
+      </c>
+      <c r="J5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!J50</f>
+        <v>GLASS_0_2</v>
+      </c>
+      <c r="K5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!K50</f>
+        <v>PP_0_1</v>
+      </c>
+      <c r="L5" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!L50</f>
+        <v>PP_0_2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B51</f>
+        <v>GLASS_100_1</v>
+      </c>
+      <c r="C6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!C51</f>
+        <v>GLASS_100_2</v>
+      </c>
+      <c r="D6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!D51</f>
+        <v>PP_100_1</v>
+      </c>
+      <c r="E6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!E51</f>
+        <v>PP_100_2</v>
+      </c>
+      <c r="F6" s="9" t="str">
+        <f aca="false">'LS Measurement arrangement'!F51</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!G51</f>
+        <v>GLASS_400_1</v>
+      </c>
+      <c r="H6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!H51</f>
+        <v>GLASS_400_2</v>
+      </c>
+      <c r="I6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!I51</f>
+        <v>PP_400_1</v>
+      </c>
+      <c r="J6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!J51</f>
+        <v>PP_400_2</v>
+      </c>
+      <c r="K6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!K51</f>
+        <v>GLASS_1000_1</v>
+      </c>
+      <c r="L6" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!L51</f>
+        <v>GLASS_1000_2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B52</f>
+        <v>PP_1000_1</v>
+      </c>
+      <c r="C7" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!C52</f>
+        <v>PP_1000_2</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="9" t="str">
+        <f aca="false">'LS Measurement arrangement'!G52</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B53</f>
+        <v>LS Vit. C</v>
+      </c>
+      <c r="C8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!C53</f>
+        <v>15% WbLS Vit. C</v>
+      </c>
+      <c r="D8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!D53</f>
+        <v>10% WbLS Vit. C</v>
+      </c>
+      <c r="E8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!E53</f>
+        <v>5% WbLS Vit. C</v>
+      </c>
+      <c r="F8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!F53</f>
+        <v>LS 10/20/14</v>
+      </c>
+      <c r="G8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!G53</f>
+        <v>WbLS-15 10/20/14</v>
+      </c>
+      <c r="H8" s="9" t="str">
+        <f aca="false">'LS Measurement arrangement'!H53</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!I53</f>
+        <v>WbLS-10 10/20/14</v>
+      </c>
+      <c r="J8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!J53</f>
+        <v>WbLS-5 10/20/14</v>
+      </c>
+      <c r="K8" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!K53</f>
+        <v>HDPE_0_1</v>
+      </c>
+      <c r="L8" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:A19"/>
@@ -1471,7 +2238,6 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q36"/>
@@ -2432,13 +3198,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:62"/>
+  <dimension ref="1:73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5690,14 +6455,6 @@
         <f aca="false">'Storage Matrix'!I74</f>
         <v>0102_1_2</v>
       </c>
-      <c r="K31" s="0" t="n">
-        <f aca="false">'Storage Matrix'!F69</f>
-        <v>0</v>
-      </c>
-      <c r="L31" s="0" t="n">
-        <f aca="false">'Storage Matrix'!G69</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
@@ -5712,7 +6469,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -6068,861 +6825,1224 @@
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
     </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1"/>
+      <c r="H44" s="9"/>
+    </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="str">
+      <c r="A46" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="9" t="str">
+        <f aca="false">B36</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C47" s="0" t="str">
+        <f aca="false">C36</f>
+        <v>0050_0_1</v>
+      </c>
+      <c r="D47" s="0" t="str">
+        <f aca="false">D36</f>
+        <v>0050_0_2</v>
+      </c>
+      <c r="E47" s="0" t="str">
+        <f aca="false">E36</f>
+        <v>0052_0_1</v>
+      </c>
+      <c r="F47" s="0" t="str">
+        <f aca="false">F36</f>
+        <v>0052_0_2</v>
+      </c>
+      <c r="G47" s="0" t="str">
+        <f aca="false">G36</f>
+        <v>0050_100_1</v>
+      </c>
+      <c r="H47" s="0" t="str">
+        <f aca="false">H36</f>
+        <v>0050_100_2</v>
+      </c>
+      <c r="I47" s="0" t="str">
+        <f aca="false">I36</f>
+        <v>0052_100_1</v>
+      </c>
+      <c r="J47" s="0" t="str">
+        <f aca="false">J36</f>
+        <v>0052_100_2</v>
+      </c>
+      <c r="K47" s="0" t="str">
+        <f aca="false">K36</f>
+        <v>0050_400_1</v>
+      </c>
+      <c r="L47" s="0" t="str">
+        <f aca="false">L36</f>
+        <v>0050_400_2</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B48" s="0" t="str">
+        <f aca="false">B37</f>
+        <v>0052_400_1</v>
+      </c>
+      <c r="C48" s="12" t="str">
+        <f aca="false">C37</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="D48" s="0" t="str">
+        <f aca="false">D37</f>
+        <v>0052_400_2</v>
+      </c>
+      <c r="E48" s="0" t="str">
+        <f aca="false">E37</f>
+        <v>0100_0_1</v>
+      </c>
+      <c r="F48" s="0" t="str">
+        <f aca="false">F37</f>
+        <v>0100_0_2</v>
+      </c>
+      <c r="G48" s="0" t="str">
+        <f aca="false">G37</f>
+        <v>0102_0_1</v>
+      </c>
+      <c r="H48" s="0" t="str">
+        <f aca="false">H37</f>
+        <v>0102_0_2</v>
+      </c>
+      <c r="I48" s="0" t="str">
+        <f aca="false">I37</f>
+        <v>0100_1_1</v>
+      </c>
+      <c r="J48" s="0" t="str">
+        <f aca="false">J37</f>
+        <v>0100_1_2</v>
+      </c>
+      <c r="K48" s="0" t="str">
+        <f aca="false">K37</f>
+        <v>0102_1_1</v>
+      </c>
+      <c r="L48" s="0" t="str">
+        <f aca="false">L37</f>
+        <v>0102_1_2</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B49" s="0" t="str">
+        <f aca="false">B38</f>
+        <v>0100_10_1</v>
+      </c>
+      <c r="C49" s="0" t="str">
+        <f aca="false">C38</f>
+        <v>0100_10_2</v>
+      </c>
+      <c r="D49" s="12" t="str">
+        <f aca="false">D38</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E49" s="0" t="str">
+        <f aca="false">E38</f>
+        <v>0102_10_1</v>
+      </c>
+      <c r="F49" s="0" t="str">
+        <f aca="false">F38</f>
+        <v>0102_10_2</v>
+      </c>
+      <c r="G49" s="0" t="str">
+        <f aca="false">G38</f>
+        <v>0100_100_1</v>
+      </c>
+      <c r="H49" s="0" t="str">
+        <f aca="false">H38</f>
+        <v>0100_100_2</v>
+      </c>
+      <c r="I49" s="0" t="str">
+        <f aca="false">I38</f>
+        <v>0102_100_1</v>
+      </c>
+      <c r="J49" s="0" t="str">
+        <f aca="false">J38</f>
+        <v>0102_100_2</v>
+      </c>
+      <c r="K49" s="0" t="str">
+        <f aca="false">K38</f>
+        <v>0100_400_1</v>
+      </c>
+      <c r="L49" s="0" t="str">
+        <f aca="false">L38</f>
+        <v>0100_400_2</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B50" s="0" t="str">
+        <f aca="false">B39</f>
+        <v>0102_400_1</v>
+      </c>
+      <c r="C50" s="0" t="str">
+        <f aca="false">C39</f>
+        <v>0102_400_2</v>
+      </c>
+      <c r="D50" s="0" t="str">
+        <f aca="false">D39</f>
+        <v>0100_1000_1</v>
+      </c>
+      <c r="E50" s="12" t="str">
+        <f aca="false">E39</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F50" s="0" t="str">
+        <f aca="false">F39</f>
+        <v>0100_1000_2</v>
+      </c>
+      <c r="G50" s="0" t="str">
+        <f aca="false">G39</f>
+        <v>0102_1000_1</v>
+      </c>
+      <c r="H50" s="0" t="str">
+        <f aca="false">H39</f>
+        <v>0102_1000_2</v>
+      </c>
+      <c r="I50" s="0" t="str">
+        <f aca="false">I39</f>
+        <v>GLASS_0_1</v>
+      </c>
+      <c r="J50" s="0" t="str">
+        <f aca="false">J39</f>
+        <v>GLASS_0_2</v>
+      </c>
+      <c r="K50" s="0" t="str">
+        <f aca="false">K39</f>
+        <v>PP_0_1</v>
+      </c>
+      <c r="L50" s="0" t="str">
+        <f aca="false">L39</f>
+        <v>PP_0_2</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B51" s="0" t="str">
+        <f aca="false">B40</f>
+        <v>GLASS_100_1</v>
+      </c>
+      <c r="C51" s="0" t="str">
+        <f aca="false">C40</f>
+        <v>GLASS_100_2</v>
+      </c>
+      <c r="D51" s="0" t="str">
+        <f aca="false">D40</f>
+        <v>PP_100_1</v>
+      </c>
+      <c r="E51" s="0" t="str">
+        <f aca="false">E40</f>
+        <v>PP_100_2</v>
+      </c>
+      <c r="F51" s="12" t="str">
+        <f aca="false">F40</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G51" s="0" t="str">
+        <f aca="false">G40</f>
+        <v>GLASS_400_1</v>
+      </c>
+      <c r="H51" s="0" t="str">
+        <f aca="false">H40</f>
+        <v>GLASS_400_2</v>
+      </c>
+      <c r="I51" s="0" t="str">
+        <f aca="false">I40</f>
+        <v>PP_400_1</v>
+      </c>
+      <c r="J51" s="0" t="str">
+        <f aca="false">J40</f>
+        <v>PP_400_2</v>
+      </c>
+      <c r="K51" s="0" t="str">
+        <f aca="false">K40</f>
+        <v>GLASS_1000_1</v>
+      </c>
+      <c r="L51" s="0" t="str">
+        <f aca="false">L40</f>
+        <v>GLASS_1000_2</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B52" s="0" t="str">
+        <f aca="false">B41</f>
+        <v>PP_1000_1</v>
+      </c>
+      <c r="C52" s="0" t="str">
+        <f aca="false">C41</f>
+        <v>PP_1000_2</v>
+      </c>
+      <c r="G52" s="12" t="str">
+        <f aca="false">G41</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B53" s="0" t="str">
+        <f aca="false">B42</f>
+        <v>LS Vit. C</v>
+      </c>
+      <c r="C53" s="0" t="str">
+        <f aca="false">C42</f>
+        <v>15% WbLS Vit. C</v>
+      </c>
+      <c r="D53" s="0" t="str">
+        <f aca="false">D42</f>
+        <v>10% WbLS Vit. C</v>
+      </c>
+      <c r="E53" s="0" t="str">
+        <f aca="false">E42</f>
+        <v>5% WbLS Vit. C</v>
+      </c>
+      <c r="F53" s="0" t="str">
+        <f aca="false">F42</f>
+        <v>LS 10/20/14</v>
+      </c>
+      <c r="G53" s="0" t="str">
+        <f aca="false">G42</f>
+        <v>WbLS-15 10/20/14</v>
+      </c>
+      <c r="H53" s="12" t="str">
+        <f aca="false">H42</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I53" s="0" t="str">
+        <f aca="false">I42</f>
+        <v>WbLS-10 10/20/14</v>
+      </c>
+      <c r="J53" s="0" t="str">
+        <f aca="false">J42</f>
+        <v>WbLS-5 10/20/14</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="L53" s="0" t="n">
+        <f aca="false">L42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="str">
         <f aca="false">A2</f>
         <v>Tray ID</v>
       </c>
-      <c r="B46" s="1" t="str">
+      <c r="B57" s="1" t="str">
         <f aca="false">B2</f>
         <v>Position 1</v>
       </c>
-      <c r="C46" s="1" t="str">
+      <c r="C57" s="1" t="str">
         <f aca="false">C2</f>
         <v>Position 2</v>
       </c>
-      <c r="D46" s="1" t="str">
+      <c r="D57" s="1" t="str">
         <f aca="false">D2</f>
         <v>Position 3</v>
       </c>
-      <c r="E46" s="1" t="str">
+      <c r="E57" s="1" t="str">
         <f aca="false">E2</f>
         <v>Position 4</v>
       </c>
-      <c r="F46" s="1" t="str">
+      <c r="F57" s="1" t="str">
         <f aca="false">F2</f>
         <v>Position 5</v>
       </c>
-      <c r="G46" s="1" t="str">
+      <c r="G57" s="1" t="str">
         <f aca="false">G2</f>
         <v>Position 6</v>
       </c>
-      <c r="H46" s="1" t="str">
+      <c r="H57" s="1" t="str">
         <f aca="false">H2</f>
         <v>Position 7</v>
       </c>
-      <c r="I46" s="1" t="str">
+      <c r="I57" s="1" t="str">
         <f aca="false">I2</f>
         <v>Position 8</v>
       </c>
-      <c r="J46" s="1" t="str">
+      <c r="J57" s="1" t="str">
         <f aca="false">J2</f>
         <v>Position 9</v>
       </c>
-      <c r="K46" s="1" t="str">
+      <c r="K57" s="1" t="str">
         <f aca="false">K2</f>
         <v>Position 10</v>
       </c>
-      <c r="L46" s="1" t="str">
+      <c r="L57" s="1" t="str">
         <f aca="false">L2</f>
         <v>Position 11</v>
       </c>
-      <c r="M46" s="1" t="str">
+      <c r="M57" s="1" t="str">
         <f aca="false">M2</f>
         <v>Position 12</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="str">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="str">
         <f aca="false">A3</f>
         <v>S1</v>
       </c>
-      <c r="B47" s="12" t="str">
+      <c r="B58" s="12" t="str">
         <f aca="false">B3</f>
         <v>EMPTY</v>
       </c>
-      <c r="C47" s="0" t="str">
+      <c r="C58" s="0" t="str">
         <f aca="false">C3</f>
         <v>0050_1F13</v>
       </c>
-      <c r="D47" s="0" t="str">
+      <c r="D58" s="0" t="str">
         <f aca="false">D3</f>
         <v>0052_1F14</v>
       </c>
-      <c r="E47" s="0" t="str">
+      <c r="E58" s="0" t="str">
         <f aca="false">E3</f>
         <v>0050_2F13</v>
       </c>
-      <c r="F47" s="0" t="str">
+      <c r="F58" s="0" t="str">
         <f aca="false">F3</f>
         <v>0052_2F14</v>
       </c>
-      <c r="G47" s="0" t="str">
+      <c r="G58" s="0" t="str">
         <f aca="false">G3</f>
         <v>0050_3F13</v>
       </c>
-      <c r="H47" s="0" t="str">
+      <c r="H58" s="0" t="str">
         <f aca="false">H3</f>
         <v>0052_3F14</v>
       </c>
-      <c r="I47" s="0" t="str">
+      <c r="I58" s="0" t="str">
         <f aca="false">I3</f>
         <v>0050_4F13</v>
       </c>
-      <c r="J47" s="0" t="str">
+      <c r="J58" s="0" t="str">
         <f aca="false">J3</f>
         <v>0052_4F14</v>
       </c>
-      <c r="K47" s="0" t="str">
+      <c r="K58" s="0" t="str">
         <f aca="false">K3</f>
         <v>0100_1F15</v>
       </c>
-      <c r="L47" s="0" t="str">
+      <c r="L58" s="0" t="str">
         <f aca="false">L3</f>
         <v>0102_1F25</v>
       </c>
-      <c r="M47" s="0" t="str">
+      <c r="M58" s="0" t="str">
         <f aca="false">M3</f>
         <v>0100_2F15</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="str">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="str">
         <f aca="false">A4</f>
         <v>S2</v>
       </c>
-      <c r="B48" s="0" t="str">
+      <c r="B59" s="0" t="str">
         <f aca="false">B4</f>
         <v>0102_2F25</v>
       </c>
-      <c r="C48" s="12" t="str">
+      <c r="C59" s="12" t="str">
         <f aca="false">C4</f>
         <v>EMPTY</v>
       </c>
-      <c r="D48" s="0" t="str">
+      <c r="D59" s="0" t="str">
         <f aca="false">D4</f>
         <v>0100_3F15</v>
       </c>
-      <c r="E48" s="0" t="str">
+      <c r="E59" s="0" t="str">
         <f aca="false">E4</f>
         <v>0102_3F25</v>
       </c>
-      <c r="F48" s="0" t="str">
+      <c r="F59" s="0" t="str">
         <f aca="false">F4</f>
         <v>0100_4F15</v>
       </c>
-      <c r="G48" s="0" t="str">
+      <c r="G59" s="0" t="str">
         <f aca="false">G4</f>
         <v>0102_4F25</v>
       </c>
-      <c r="H48" s="0" t="str">
+      <c r="H59" s="0" t="str">
         <f aca="false">H4</f>
         <v>0140_1F23</v>
       </c>
-      <c r="I48" s="0" t="str">
+      <c r="I59" s="0" t="str">
         <f aca="false">I4</f>
         <v>0142_1F33</v>
       </c>
-      <c r="J48" s="0" t="str">
+      <c r="J59" s="0" t="str">
         <f aca="false">J4</f>
         <v>0140_2F23</v>
       </c>
-      <c r="K48" s="0" t="str">
+      <c r="K59" s="0" t="str">
         <f aca="false">K4</f>
         <v>0142_2F33</v>
       </c>
-      <c r="L48" s="0" t="str">
+      <c r="L59" s="0" t="str">
         <f aca="false">L4</f>
         <v>0140_3F23</v>
       </c>
-      <c r="M48" s="0" t="str">
+      <c r="M59" s="0" t="str">
         <f aca="false">M4</f>
         <v>0142_3F33</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="str">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="str">
         <f aca="false">A5</f>
         <v>S3</v>
       </c>
-      <c r="B49" s="0" t="str">
+      <c r="B60" s="0" t="str">
         <f aca="false">B5</f>
         <v>0140_4F23</v>
       </c>
-      <c r="C49" s="0" t="str">
+      <c r="C60" s="0" t="str">
         <f aca="false">C5</f>
         <v>0142_4F33</v>
       </c>
-      <c r="D49" s="12" t="str">
+      <c r="D60" s="12" t="str">
         <f aca="false">D5</f>
         <v>EMPTY</v>
       </c>
-      <c r="E49" s="0" t="str">
+      <c r="E60" s="0" t="str">
         <f aca="false">E5</f>
         <v>1000_1F34</v>
       </c>
-      <c r="F49" s="0" t="str">
+      <c r="F60" s="0" t="str">
         <f aca="false">F5</f>
         <v>1002_1F35</v>
       </c>
-      <c r="G49" s="0" t="str">
+      <c r="G60" s="0" t="str">
         <f aca="false">G5</f>
         <v>1000_2F34</v>
       </c>
-      <c r="H49" s="0" t="str">
+      <c r="H60" s="0" t="str">
         <f aca="false">H5</f>
         <v>1002_2F35</v>
       </c>
-      <c r="I49" s="0" t="str">
+      <c r="I60" s="0" t="str">
         <f aca="false">I5</f>
         <v>1000_3F34</v>
       </c>
-      <c r="J49" s="0" t="str">
+      <c r="J60" s="0" t="str">
         <f aca="false">J5</f>
         <v>1002_3F35</v>
       </c>
-      <c r="K49" s="0" t="str">
+      <c r="K60" s="0" t="str">
         <f aca="false">K5</f>
         <v>1000_4F34</v>
       </c>
-      <c r="L49" s="0" t="str">
+      <c r="L60" s="0" t="str">
         <f aca="false">L5</f>
         <v>1002_4F35</v>
       </c>
-      <c r="M49" s="0" t="str">
+      <c r="M60" s="0" t="str">
         <f aca="false">M5</f>
         <v>0050_1R13</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="str">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="str">
         <f aca="false">A6</f>
         <v>S4</v>
       </c>
-      <c r="B50" s="0" t="str">
+      <c r="B61" s="0" t="str">
         <f aca="false">B6</f>
         <v>0052_1R14</v>
       </c>
-      <c r="C50" s="0" t="str">
+      <c r="C61" s="0" t="str">
         <f aca="false">C6</f>
         <v>0050_2R13</v>
       </c>
-      <c r="D50" s="0" t="str">
+      <c r="D61" s="0" t="str">
         <f aca="false">D6</f>
         <v>0052_2R14</v>
       </c>
-      <c r="E50" s="12" t="str">
+      <c r="E61" s="12" t="str">
         <f aca="false">E6</f>
         <v>EMPTY</v>
       </c>
-      <c r="F50" s="0" t="str">
+      <c r="F61" s="0" t="str">
         <f aca="false">F6</f>
         <v>0050_3R13</v>
       </c>
-      <c r="G50" s="0" t="str">
+      <c r="G61" s="0" t="str">
         <f aca="false">G6</f>
         <v>0052_3R14</v>
       </c>
-      <c r="H50" s="0" t="str">
+      <c r="H61" s="0" t="str">
         <f aca="false">H6</f>
         <v>0050_4R13</v>
       </c>
-      <c r="I50" s="0" t="str">
+      <c r="I61" s="0" t="str">
         <f aca="false">I6</f>
         <v>0052_4R14</v>
       </c>
-      <c r="J50" s="0" t="str">
+      <c r="J61" s="0" t="str">
         <f aca="false">J6</f>
         <v>0100_1R15</v>
       </c>
-      <c r="K50" s="0" t="str">
+      <c r="K61" s="0" t="str">
         <f aca="false">K6</f>
         <v>0102_1R25</v>
       </c>
-      <c r="L50" s="0" t="str">
+      <c r="L61" s="0" t="str">
         <f aca="false">L6</f>
         <v>0100_2R15</v>
       </c>
-      <c r="M50" s="0" t="str">
+      <c r="M61" s="0" t="str">
         <f aca="false">M6</f>
         <v>0102_2R25</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="str">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="str">
         <f aca="false">A7</f>
         <v>S5</v>
       </c>
-      <c r="B51" s="0" t="str">
+      <c r="B62" s="0" t="str">
         <f aca="false">B7</f>
         <v>0100_3R15</v>
       </c>
-      <c r="C51" s="0" t="str">
+      <c r="C62" s="0" t="str">
         <f aca="false">C7</f>
         <v>0102_3R25</v>
       </c>
-      <c r="D51" s="0" t="str">
+      <c r="D62" s="0" t="str">
         <f aca="false">D7</f>
         <v>0100_4R15</v>
       </c>
-      <c r="E51" s="0" t="str">
+      <c r="E62" s="0" t="str">
         <f aca="false">E7</f>
         <v>0102_4R25</v>
       </c>
-      <c r="F51" s="12" t="str">
+      <c r="F62" s="12" t="str">
         <f aca="false">F7</f>
         <v>EMPTY</v>
       </c>
-      <c r="G51" s="0" t="str">
+      <c r="G62" s="0" t="str">
         <f aca="false">G7</f>
         <v>0140_1R23</v>
       </c>
-      <c r="H51" s="0" t="str">
+      <c r="H62" s="0" t="str">
         <f aca="false">H7</f>
         <v>0142_1R33</v>
       </c>
-      <c r="I51" s="0" t="str">
+      <c r="I62" s="0" t="str">
         <f aca="false">I7</f>
         <v>0140_2R23</v>
       </c>
-      <c r="J51" s="0" t="str">
+      <c r="J62" s="0" t="str">
         <f aca="false">J7</f>
         <v>0142_2R33</v>
       </c>
-      <c r="K51" s="0" t="str">
+      <c r="K62" s="0" t="str">
         <f aca="false">K7</f>
         <v>0140_3R23</v>
       </c>
-      <c r="L51" s="0" t="str">
+      <c r="L62" s="0" t="str">
         <f aca="false">L7</f>
         <v>0142_3R33</v>
       </c>
-      <c r="M51" s="0" t="str">
+      <c r="M62" s="0" t="str">
         <f aca="false">M7</f>
         <v>0140_4R23</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="str">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="str">
         <f aca="false">A8</f>
         <v>S6</v>
       </c>
-      <c r="B52" s="0" t="str">
+      <c r="B63" s="0" t="str">
         <f aca="false">B8</f>
         <v>0142_4R33</v>
       </c>
-      <c r="C52" s="0" t="str">
+      <c r="C63" s="0" t="str">
         <f aca="false">C8</f>
         <v>1000_1R34</v>
       </c>
-      <c r="D52" s="0" t="str">
+      <c r="D63" s="0" t="str">
         <f aca="false">D8</f>
         <v>1002_1R35</v>
       </c>
-      <c r="E52" s="0" t="str">
+      <c r="E63" s="0" t="str">
         <f aca="false">E8</f>
         <v>1000_2R34</v>
       </c>
-      <c r="F52" s="0" t="str">
+      <c r="F63" s="0" t="str">
         <f aca="false">F8</f>
         <v>1002_2R35</v>
       </c>
-      <c r="G52" s="12" t="str">
+      <c r="G63" s="12" t="str">
         <f aca="false">G8</f>
         <v>EMPTY</v>
       </c>
-      <c r="H52" s="0" t="str">
+      <c r="H63" s="0" t="str">
         <f aca="false">H8</f>
         <v>1000_3R34</v>
       </c>
-      <c r="I52" s="0" t="str">
+      <c r="I63" s="0" t="str">
         <f aca="false">I8</f>
         <v>1002_3R35</v>
       </c>
-      <c r="J52" s="0" t="str">
+      <c r="J63" s="0" t="str">
         <f aca="false">J8</f>
         <v>1000_4R34</v>
       </c>
-      <c r="K52" s="0" t="str">
+      <c r="K63" s="0" t="str">
         <f aca="false">K8</f>
         <v>1002_4R35</v>
       </c>
-      <c r="L52" s="0" t="str">
+      <c r="L63" s="0" t="str">
         <f aca="false">L8</f>
         <v>0050_FPMT</v>
       </c>
-      <c r="M52" s="0" t="str">
+      <c r="M63" s="0" t="str">
         <f aca="false">M8</f>
         <v>0050_RPMT</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="str">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="str">
         <f aca="false">A9</f>
         <v>S7</v>
       </c>
-      <c r="B53" s="0" t="str">
+      <c r="B64" s="0" t="str">
         <f aca="false">B9</f>
         <v>0050_1F11</v>
       </c>
-      <c r="C53" s="0" t="str">
+      <c r="C64" s="0" t="str">
         <f aca="false">C9</f>
         <v>0052_1F12</v>
       </c>
-      <c r="D53" s="0" t="str">
+      <c r="D64" s="0" t="str">
         <f aca="false">D9</f>
         <v>0050_2F11</v>
       </c>
-      <c r="E53" s="0" t="str">
+      <c r="E64" s="0" t="str">
         <f aca="false">E9</f>
         <v>0052_2F12</v>
       </c>
-      <c r="F53" s="0" t="str">
+      <c r="F64" s="0" t="str">
         <f aca="false">F9</f>
         <v>0050_3F11</v>
       </c>
-      <c r="G53" s="0" t="str">
+      <c r="G64" s="0" t="str">
         <f aca="false">G9</f>
         <v>0052_3F12</v>
       </c>
-      <c r="H53" s="12" t="str">
+      <c r="H64" s="12" t="str">
         <f aca="false">H9</f>
         <v>EMPTY</v>
       </c>
-      <c r="I53" s="0" t="str">
+      <c r="I64" s="0" t="str">
         <f aca="false">I9</f>
         <v>0050_4F11</v>
       </c>
-      <c r="J53" s="0" t="str">
+      <c r="J64" s="0" t="str">
         <f aca="false">J9</f>
         <v>0052_4F12</v>
       </c>
-      <c r="K53" s="0" t="str">
+      <c r="K64" s="0" t="str">
         <f aca="false">K9</f>
         <v>0100_1F22</v>
       </c>
-      <c r="L53" s="0" t="str">
+      <c r="L64" s="0" t="str">
         <f aca="false">L9</f>
         <v>0102_1F21</v>
       </c>
-      <c r="M53" s="0" t="str">
+      <c r="M64" s="0" t="str">
         <f aca="false">M9</f>
         <v>0100_2F22</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="str">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="str">
         <f aca="false">A10</f>
         <v>S8</v>
       </c>
-      <c r="B54" s="0" t="str">
+      <c r="B65" s="0" t="str">
         <f aca="false">B10</f>
         <v>0102_2F21</v>
       </c>
-      <c r="C54" s="0" t="str">
+      <c r="C65" s="0" t="str">
         <f aca="false">C10</f>
         <v>0100_3F22</v>
       </c>
-      <c r="D54" s="0" t="str">
+      <c r="D65" s="0" t="str">
         <f aca="false">D10</f>
         <v>0102_3F21</v>
       </c>
-      <c r="E54" s="0" t="str">
+      <c r="E65" s="0" t="str">
         <f aca="false">E10</f>
         <v>0100_4F22</v>
       </c>
-      <c r="F54" s="0" t="str">
+      <c r="F65" s="0" t="str">
         <f aca="false">F10</f>
         <v>0102_4F21</v>
       </c>
-      <c r="G54" s="0" t="str">
+      <c r="G65" s="0" t="str">
         <f aca="false">G10</f>
         <v>0140_1F31</v>
       </c>
-      <c r="H54" s="0" t="str">
+      <c r="H65" s="0" t="str">
         <f aca="false">H10</f>
         <v>0142_1F26</v>
       </c>
-      <c r="I54" s="12" t="str">
+      <c r="I65" s="12" t="str">
         <f aca="false">I10</f>
         <v>EMPTY</v>
       </c>
-      <c r="J54" s="0" t="str">
+      <c r="J65" s="0" t="str">
         <f aca="false">J10</f>
         <v>0140_2F31</v>
       </c>
-      <c r="K54" s="0" t="str">
+      <c r="K65" s="0" t="str">
         <f aca="false">K10</f>
         <v>0142_2F26</v>
       </c>
-      <c r="L54" s="0" t="str">
+      <c r="L65" s="0" t="str">
         <f aca="false">L10</f>
         <v>0140_3F31</v>
       </c>
-      <c r="M54" s="0" t="str">
+      <c r="M65" s="0" t="str">
         <f aca="false">M10</f>
         <v>0142_3F26</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="str">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="str">
         <f aca="false">A11</f>
         <v>S9</v>
       </c>
-      <c r="B55" s="0" t="str">
+      <c r="B66" s="0" t="str">
         <f aca="false">B11</f>
         <v>0140_4F31</v>
       </c>
-      <c r="C55" s="0" t="str">
+      <c r="C66" s="0" t="str">
         <f aca="false">C11</f>
         <v>0142_4F26</v>
       </c>
-      <c r="D55" s="0" t="str">
+      <c r="D66" s="0" t="str">
         <f aca="false">D11</f>
         <v>1000_1F36</v>
       </c>
-      <c r="E55" s="0" t="str">
+      <c r="E66" s="0" t="str">
         <f aca="false">E11</f>
         <v>1002_1F32</v>
       </c>
-      <c r="F55" s="0" t="str">
+      <c r="F66" s="0" t="str">
         <f aca="false">F11</f>
         <v>1000_2F36</v>
       </c>
-      <c r="G55" s="0" t="str">
+      <c r="G66" s="0" t="str">
         <f aca="false">G11</f>
         <v>1002_2F32</v>
       </c>
-      <c r="H55" s="0" t="str">
+      <c r="H66" s="0" t="str">
         <f aca="false">H11</f>
         <v>1000_3F36</v>
       </c>
-      <c r="I55" s="0" t="str">
+      <c r="I66" s="0" t="str">
         <f aca="false">I11</f>
         <v>1002_3F32</v>
       </c>
-      <c r="J55" s="12" t="str">
+      <c r="J66" s="12" t="str">
         <f aca="false">J11</f>
         <v>EMPTY</v>
       </c>
-      <c r="K55" s="0" t="str">
+      <c r="K66" s="0" t="str">
         <f aca="false">K11</f>
         <v>1000_4F36</v>
       </c>
-      <c r="L55" s="0" t="str">
+      <c r="L66" s="0" t="str">
         <f aca="false">L11</f>
         <v>1002_4F32</v>
       </c>
-      <c r="M55" s="0" t="str">
+      <c r="M66" s="0" t="str">
         <f aca="false">M11</f>
         <v>0050_1R11</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="str">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="str">
         <f aca="false">A12</f>
         <v>S10</v>
       </c>
-      <c r="B56" s="0" t="str">
+      <c r="B67" s="0" t="str">
         <f aca="false">B12</f>
         <v>0052_1R12</v>
       </c>
-      <c r="C56" s="0" t="str">
+      <c r="C67" s="0" t="str">
         <f aca="false">C12</f>
         <v>0050_2R11</v>
       </c>
-      <c r="D56" s="0" t="str">
+      <c r="D67" s="0" t="str">
         <f aca="false">D12</f>
         <v>0052_2R12</v>
       </c>
-      <c r="E56" s="0" t="str">
+      <c r="E67" s="0" t="str">
         <f aca="false">E12</f>
         <v>0050_3R11</v>
       </c>
-      <c r="F56" s="0" t="str">
+      <c r="F67" s="0" t="str">
         <f aca="false">F12</f>
         <v>0052_3R12</v>
       </c>
-      <c r="G56" s="0" t="str">
+      <c r="G67" s="0" t="str">
         <f aca="false">G12</f>
         <v>0050_4R11</v>
       </c>
-      <c r="H56" s="0" t="str">
+      <c r="H67" s="0" t="str">
         <f aca="false">H12</f>
         <v>0052_4R12</v>
       </c>
-      <c r="I56" s="0" t="str">
+      <c r="I67" s="0" t="str">
         <f aca="false">I12</f>
         <v>0100_1R22</v>
       </c>
-      <c r="J56" s="0" t="str">
+      <c r="J67" s="0" t="str">
         <f aca="false">J12</f>
         <v>0102_1R21</v>
       </c>
-      <c r="K56" s="12" t="str">
+      <c r="K67" s="12" t="str">
         <f aca="false">K12</f>
         <v>EMPTY</v>
       </c>
-      <c r="L56" s="0" t="str">
+      <c r="L67" s="0" t="str">
         <f aca="false">L12</f>
         <v>0100_2R22</v>
       </c>
-      <c r="M56" s="0" t="str">
+      <c r="M67" s="0" t="str">
         <f aca="false">M12</f>
         <v>0102_2R21</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="str">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="str">
         <f aca="false">A13</f>
         <v>S11</v>
       </c>
-      <c r="B57" s="0" t="str">
+      <c r="B68" s="0" t="str">
         <f aca="false">B13</f>
         <v>0100_3R22</v>
       </c>
-      <c r="C57" s="0" t="str">
+      <c r="C68" s="0" t="str">
         <f aca="false">C13</f>
         <v>0102_3R21</v>
       </c>
-      <c r="D57" s="0" t="str">
+      <c r="D68" s="0" t="str">
         <f aca="false">D13</f>
         <v>0100_4R22</v>
       </c>
-      <c r="E57" s="0" t="str">
+      <c r="E68" s="0" t="str">
         <f aca="false">E13</f>
         <v>0102_4R21</v>
       </c>
-      <c r="F57" s="0" t="str">
+      <c r="F68" s="0" t="str">
         <f aca="false">F13</f>
         <v>0140_1R31</v>
       </c>
-      <c r="G57" s="0" t="str">
+      <c r="G68" s="0" t="str">
         <f aca="false">G13</f>
         <v>0142_1R26</v>
       </c>
-      <c r="H57" s="0" t="str">
+      <c r="H68" s="0" t="str">
         <f aca="false">H13</f>
         <v>0140_2R31</v>
       </c>
-      <c r="I57" s="0" t="str">
+      <c r="I68" s="0" t="str">
         <f aca="false">I13</f>
         <v>0142_2R26</v>
       </c>
-      <c r="J57" s="0" t="str">
+      <c r="J68" s="0" t="str">
         <f aca="false">J13</f>
         <v>0140_3R31</v>
       </c>
-      <c r="K57" s="0" t="str">
+      <c r="K68" s="0" t="str">
         <f aca="false">K13</f>
         <v>0142_3R26</v>
       </c>
-      <c r="L57" s="12" t="str">
+      <c r="L68" s="12" t="str">
         <f aca="false">L13</f>
         <v>EMPTY</v>
       </c>
-      <c r="M57" s="0" t="str">
+      <c r="M68" s="0" t="str">
         <f aca="false">M13</f>
         <v>0140_4R31</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="str">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="str">
         <f aca="false">A14</f>
         <v>S12</v>
       </c>
-      <c r="B58" s="0" t="str">
+      <c r="B69" s="0" t="str">
         <f aca="false">B14</f>
         <v>0142_4R26</v>
       </c>
-      <c r="C58" s="0" t="str">
+      <c r="C69" s="0" t="str">
         <f aca="false">C14</f>
         <v>1000_1R36</v>
       </c>
-      <c r="D58" s="0" t="str">
+      <c r="D69" s="0" t="str">
         <f aca="false">D14</f>
         <v>1002_1R32</v>
       </c>
-      <c r="E58" s="0" t="str">
+      <c r="E69" s="0" t="str">
         <f aca="false">E14</f>
         <v>1000_2R36</v>
       </c>
-      <c r="F58" s="0" t="str">
+      <c r="F69" s="0" t="str">
         <f aca="false">F14</f>
         <v>1002_2R32</v>
       </c>
-      <c r="G58" s="0" t="str">
+      <c r="G69" s="0" t="str">
         <f aca="false">G14</f>
         <v>1000_3R36</v>
       </c>
-      <c r="H58" s="0" t="str">
+      <c r="H69" s="0" t="str">
         <f aca="false">H14</f>
         <v>1002_3R32</v>
       </c>
-      <c r="I58" s="0" t="str">
+      <c r="I69" s="0" t="str">
         <f aca="false">I14</f>
         <v>1000_4R36</v>
       </c>
-      <c r="J58" s="0" t="str">
+      <c r="J69" s="0" t="str">
         <f aca="false">J14</f>
         <v>1002_4R32</v>
       </c>
-      <c r="K58" s="0" t="str">
+      <c r="K69" s="0" t="str">
         <f aca="false">K14</f>
         <v>0050_1F16</v>
       </c>
-      <c r="L58" s="0" t="str">
+      <c r="L69" s="0" t="str">
         <f aca="false">L14</f>
         <v>0052_1F17</v>
       </c>
-      <c r="M58" s="12" t="str">
+      <c r="M69" s="12" t="str">
         <f aca="false">M14</f>
         <v>EMPTY</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="str">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="str">
         <f aca="false">A17</f>
         <v>S13</v>
       </c>
-      <c r="B59" s="12" t="str">
+      <c r="B70" s="12" t="str">
         <f aca="false">B17</f>
         <v>EMPTY</v>
       </c>
-      <c r="C59" s="0" t="str">
+      <c r="C70" s="0" t="str">
         <f aca="false">C17</f>
         <v>0050_2F16</v>
       </c>
-      <c r="D59" s="12" t="str">
+      <c r="D70" s="12" t="str">
         <f aca="false">D17</f>
         <v>EMPTY</v>
       </c>
-      <c r="E59" s="0" t="str">
+      <c r="E70" s="0" t="str">
         <f aca="false">E17</f>
         <v>0052_2F17</v>
       </c>
-      <c r="F59" s="0" t="str">
+      <c r="F70" s="0" t="str">
         <f aca="false">F17</f>
         <v>0050_3F16</v>
       </c>
-      <c r="G59" s="0" t="str">
+      <c r="G70" s="0" t="str">
         <f aca="false">G17</f>
         <v>0052_3F17</v>
       </c>
-      <c r="H59" s="0" t="str">
+      <c r="H70" s="0" t="str">
         <f aca="false">H17</f>
         <v>0050_4F16</v>
       </c>
-      <c r="I59" s="0" t="str">
+      <c r="I70" s="0" t="str">
         <f aca="false">I17</f>
         <v>0052_4F17</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="str">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="str">
         <f aca="false">A16</f>
         <v>S14</v>
       </c>
-      <c r="B60" s="12" t="str">
+      <c r="B71" s="12" t="str">
         <f aca="false">B16</f>
         <v>EMPTY</v>
       </c>
-      <c r="E60" s="12" t="str">
+      <c r="E71" s="12" t="str">
         <f aca="false">E16</f>
         <v>EMPTY</v>
       </c>
-      <c r="H60" s="0" t="str">
+      <c r="H71" s="0" t="str">
         <f aca="false">H16</f>
         <v>0050_1R16</v>
       </c>
-      <c r="I60" s="0" t="str">
+      <c r="I71" s="0" t="str">
         <f aca="false">I16</f>
         <v>0052_1R17</v>
       </c>
-      <c r="J60" s="0" t="str">
+      <c r="J71" s="0" t="str">
         <f aca="false">J16</f>
         <v>0050_2R16</v>
       </c>
-      <c r="K60" s="0" t="str">
+      <c r="K71" s="0" t="str">
         <f aca="false">K16</f>
         <v>0052_2R17</v>
       </c>
-      <c r="L60" s="0" t="str">
+      <c r="L71" s="0" t="str">
         <f aca="false">L16</f>
         <v>0050_3R16</v>
       </c>
-      <c r="M60" s="0" t="str">
+      <c r="M71" s="0" t="str">
         <f aca="false">M16</f>
         <v>0052_3R17</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="str">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="str">
         <f aca="false">A15</f>
         <v>S15</v>
       </c>
-      <c r="B61" s="12" t="str">
+      <c r="B72" s="12" t="str">
         <f aca="false">B15</f>
         <v>EMPTY</v>
       </c>
-      <c r="C61" s="0" t="str">
+      <c r="C72" s="0" t="str">
         <f aca="false">C15</f>
         <v>0050_4R16</v>
       </c>
-      <c r="D61" s="0" t="str">
+      <c r="D72" s="0" t="str">
         <f aca="false">D15</f>
         <v>0052_4R17</v>
       </c>
-      <c r="F61" s="12" t="str">
+      <c r="F72" s="12" t="str">
         <f aca="false">F15</f>
         <v>EMPTY</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="str">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="10" t="str">
         <f aca="false">A18</f>
         <v>R1</v>
       </c>
-      <c r="B62" s="7" t="str">
+      <c r="B73" s="7" t="str">
         <f aca="false">B18</f>
         <v>0050_REF1</v>
       </c>
-      <c r="C62" s="7" t="str">
+      <c r="C73" s="7" t="str">
         <f aca="false">C18</f>
         <v>0052_REF1</v>
       </c>
-      <c r="D62" s="7" t="str">
+      <c r="D73" s="7" t="str">
         <f aca="false">D18</f>
         <v>0100_REF1</v>
       </c>
-      <c r="E62" s="7" t="str">
+      <c r="E73" s="7" t="str">
         <f aca="false">E18</f>
         <v>0102_REF1</v>
       </c>
-      <c r="F62" s="7" t="str">
+      <c r="F73" s="7" t="str">
         <f aca="false">F18</f>
         <v>0200_REF1</v>
       </c>
-      <c r="G62" s="7" t="str">
+      <c r="G73" s="7" t="str">
         <f aca="false">G18</f>
         <v>0202_REF1</v>
       </c>
-      <c r="H62" s="7" t="str">
+      <c r="H73" s="7" t="str">
         <f aca="false">H18</f>
         <v>1000_REF1</v>
       </c>
-      <c r="I62" s="7" t="str">
+      <c r="I73" s="7" t="str">
         <f aca="false">I18</f>
         <v>1002_REF1</v>
       </c>
-      <c r="J62" s="7" t="str">
+      <c r="J73" s="7" t="str">
         <f aca="false">J18</f>
         <v>0050_REF2</v>
       </c>
-      <c r="K62" s="7" t="str">
+      <c r="K73" s="7" t="str">
         <f aca="false">K18</f>
         <v>0052_REF2</v>
       </c>
-      <c r="L62" s="7" t="str">
+      <c r="L73" s="7" t="str">
         <f aca="false">L18</f>
         <v>0100_REF2</v>
       </c>
-      <c r="M62" s="7" t="str">
+      <c r="M73" s="7" t="str">
         <f aca="false">M18</f>
         <v>0102_REF2</v>
       </c>
@@ -6941,7 +8061,6 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K80"/>
@@ -6958,12 +8077,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>0</v>
@@ -7216,12 +8335,12 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0</v>
@@ -7474,12 +8593,12 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>0</v>
@@ -7732,12 +8851,12 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>0</v>
@@ -7990,12 +9109,12 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>0</v>
@@ -8033,10 +9152,10 @@
         <v>0</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D57" s="6" t="str">
         <f aca="false">HolderMatrix!B30</f>
@@ -8047,10 +9166,10 @@
         <v>0050_RPMT</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>184</v>
@@ -8188,12 +9307,12 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B70" s="1" t="n">
         <v>0</v>
@@ -8231,34 +9350,34 @@
         <v>0</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8266,34 +9385,34 @@
         <v>1</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="J72" s="7" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="K72" s="7" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8301,28 +9420,28 @@
         <v>2</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8330,34 +9449,34 @@
         <v>3</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8365,34 +9484,34 @@
         <v>4</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="J75" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="K75" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8400,16 +9519,16 @@
         <v>5</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8432,28 +9551,28 @@
         <v>7</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I78" s="13" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
@@ -8502,7 +9621,6 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G19"/>
@@ -8518,22 +9636,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8607,37 +9725,1307 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>325</v>
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C3</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D3</f>
+        <v>0052_1F14</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E3</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F3</f>
+        <v>0052_2F14</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G3</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H3</f>
+        <v>0052_3F14</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I3</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J3</f>
+        <v>0052_4F14</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K3</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L3</f>
+        <v>0102_1F25</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M3</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B4</f>
+        <v>0102_2F25</v>
+      </c>
+      <c r="C3" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!C4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D4</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E4</f>
+        <v>0102_3F25</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F4</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G4</f>
+        <v>0102_4F25</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H4</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I4</f>
+        <v>0142_1F33</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J4</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K4</f>
+        <v>0142_2F33</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L4</f>
+        <v>0140_3F23</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M4</f>
+        <v>0142_3F33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B5</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C5</f>
+        <v>0142_4F33</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!D5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E5</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F5</f>
+        <v>1002_1F35</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G5</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H5</f>
+        <v>1002_2F35</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I5</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J5</f>
+        <v>1002_3F35</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K5</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L5</f>
+        <v>1002_4F35</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M5</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B6</f>
+        <v>0052_1R14</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C6</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D6</f>
+        <v>0052_2R14</v>
+      </c>
+      <c r="E5" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!E6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F6</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G6</f>
+        <v>0052_3R14</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H6</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I6</f>
+        <v>0052_4R14</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J6</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K6</f>
+        <v>0102_1R25</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L6</f>
+        <v>0100_2R15</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M6</f>
+        <v>0102_2R25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B7</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C7</f>
+        <v>0102_3R25</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D7</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E7</f>
+        <v>0102_4R25</v>
+      </c>
+      <c r="F6" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!F7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G7</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H7</f>
+        <v>0142_1R33</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I7</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J7</f>
+        <v>0142_2R33</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K7</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L7</f>
+        <v>0142_3R33</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M7</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B8</f>
+        <v>0142_4R33</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C8</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D8</f>
+        <v>1002_1R35</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E8</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F8</f>
+        <v>1002_2R35</v>
+      </c>
+      <c r="G7" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!G8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H8</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="I7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I8</f>
+        <v>1002_3R35</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J8</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="K7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K8</f>
+        <v>1002_4R35</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L8</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M8</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B9</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C9</f>
+        <v>0052_1F12</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D9</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E9</f>
+        <v>0052_2F12</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F9</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G9</f>
+        <v>0052_3F12</v>
+      </c>
+      <c r="H8" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!H9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I9</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J9</f>
+        <v>0052_4F12</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K9</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L9</f>
+        <v>0102_1F21</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M9</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B10</f>
+        <v>0102_2F21</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C10</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D10</f>
+        <v>0102_3F21</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E10</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F10</f>
+        <v>0102_4F21</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G10</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H10</f>
+        <v>0142_1F26</v>
+      </c>
+      <c r="I9" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!I10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J10</f>
+        <v>0140_2F31</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K10</f>
+        <v>0142_2F26</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L10</f>
+        <v>0140_3F31</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M10</f>
+        <v>0142_3F26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B11</f>
+        <v>0140_4F31</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C11</f>
+        <v>0142_4F26</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D11</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E11</f>
+        <v>1002_1F32</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F11</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="G10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G11</f>
+        <v>1002_2F32</v>
+      </c>
+      <c r="H10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H11</f>
+        <v>1000_3F36</v>
+      </c>
+      <c r="I10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I11</f>
+        <v>1002_3F32</v>
+      </c>
+      <c r="J10" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!J11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="K10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K11</f>
+        <v>1000_4F36</v>
+      </c>
+      <c r="L10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L11</f>
+        <v>1002_4F32</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M11</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B12</f>
+        <v>0052_1R12</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C12</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="D11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D12</f>
+        <v>0052_2R12</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E12</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="F11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F12</f>
+        <v>0052_3R12</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G12</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="H11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H12</f>
+        <v>0052_4R12</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I12</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="J11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J12</f>
+        <v>0102_1R21</v>
+      </c>
+      <c r="K11" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!K12</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L12</f>
+        <v>0100_2R22</v>
+      </c>
+      <c r="M11" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M12</f>
+        <v>0102_2R21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B13</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C13</f>
+        <v>0102_3R21</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D13</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E13</f>
+        <v>0102_4R21</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F13</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G13</f>
+        <v>0142_1R26</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H13</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="I12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I13</f>
+        <v>0142_2R26</v>
+      </c>
+      <c r="J12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J13</f>
+        <v>0140_3R31</v>
+      </c>
+      <c r="K12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K13</f>
+        <v>0142_3R26</v>
+      </c>
+      <c r="L12" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!L13</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M12" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M13</f>
+        <v>0140_4R31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B14</f>
+        <v>0142_4R26</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C14</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D14</f>
+        <v>1002_1R32</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E14</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="F13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F14</f>
+        <v>1002_2R32</v>
+      </c>
+      <c r="G13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G14</f>
+        <v>1000_3R36</v>
+      </c>
+      <c r="H13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H14</f>
+        <v>1002_3R32</v>
+      </c>
+      <c r="I13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I14</f>
+        <v>1000_4R36</v>
+      </c>
+      <c r="J13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J14</f>
+        <v>1002_4R32</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K14</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="L13" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L14</f>
+        <v>0052_1F17</v>
+      </c>
+      <c r="M13" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!M14</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C15</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="D14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D15</f>
+        <v>0052_4R17</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E15</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F14" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!F15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G15</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H15</f>
+        <v>0100_3R27</v>
+      </c>
+      <c r="I14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I15</f>
+        <v>0100_4R27</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J15</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K15</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L15</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M14" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M15</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C16</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D16</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!E16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F16</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G16</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H16</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="I15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I16</f>
+        <v>0052_1R17</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J16</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="K15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K16</f>
+        <v>0052_2R17</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L16</f>
+        <v>0050_3R16</v>
+      </c>
+      <c r="M15" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M16</f>
+        <v>0052_3R17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B16" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!B17</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C17</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D16" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!D17</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E17</f>
+        <v>0052_2F17</v>
+      </c>
+      <c r="F16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F17</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G17</f>
+        <v>0052_3F17</v>
+      </c>
+      <c r="H16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H17</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="I16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I17</f>
+        <v>0052_4F17</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J17</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K17</f>
+        <v>0100_2F27</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L17</f>
+        <v>0100_3F27</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!M17</f>
+        <v>0100_4F27</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!B18</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!C18</f>
+        <v>0052_REF1</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!D18</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!E18</f>
+        <v>0102_REF1</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!F18</f>
+        <v>0200_REF1</v>
+      </c>
+      <c r="G17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!G18</f>
+        <v>0202_REF1</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!H18</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!I18</f>
+        <v>1002_REF1</v>
+      </c>
+      <c r="J17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!J18</f>
+        <v>0050_REF2</v>
+      </c>
+      <c r="K17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!K18</f>
+        <v>0052_REF2</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!L18</f>
+        <v>0100_REF2</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f aca="false">'LS Measurement arrangement'!M18</f>
+        <v>0102_REF2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C23</f>
+        <v>0050_0_1</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D23</f>
+        <v>0050_0_2</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E23</f>
+        <v>0052_0_1</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F23</f>
+        <v>0052_0_2</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G23</f>
+        <v>0050_100_1</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H23</f>
+        <v>0050_100_2</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I23</f>
+        <v>0052_100_1</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J23</f>
+        <v>0052_100_2</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K23</f>
+        <v>0050_400_1</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L23</f>
+        <v>0050_400_2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B24</f>
+        <v>0052_400_1</v>
+      </c>
+      <c r="C3" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!C24</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D24</f>
+        <v>0052_400_2</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E24</f>
+        <v>0100_0_1</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F24</f>
+        <v>0100_0_2</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G24</f>
+        <v>0102_0_1</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H24</f>
+        <v>0102_0_2</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I24</f>
+        <v>0100_1_1</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J24</f>
+        <v>0100_1_2</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K24</f>
+        <v>0102_1_1</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L24</f>
+        <v>0102_1_2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B25</f>
+        <v>0100_10_1</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C25</f>
+        <v>0100_10_2</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!D25</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E25</f>
+        <v>0102_10_1</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F25</f>
+        <v>0102_10_2</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G25</f>
+        <v>0100_100_1</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H25</f>
+        <v>0100_100_2</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I25</f>
+        <v>0102_100_1</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J25</f>
+        <v>0102_100_2</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K25</f>
+        <v>0100_400_1</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!L25</f>
+        <v>0100_400_2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!B26</f>
+        <v>0102_400_1</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C26</f>
+        <v>0102_400_2</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D26</f>
+        <v>0100_1000_1</v>
+      </c>
+      <c r="E5" s="12" t="str">
+        <f aca="false">'LS Measurement arrangement'!E26</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F26</f>
+        <v>0100_1000_2</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G26</f>
+        <v>0102_1000_1</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H26</f>
+        <v>0102_1000_2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!C31</f>
+        <v>0100_0_1</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!D31</f>
+        <v>0100_0_2</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!E31</f>
+        <v>0102_0_1</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!F31</f>
+        <v>0102_0_2</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!G31</f>
+        <v>0100_1_1</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!H31</f>
+        <v>0100_1_2</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!I31</f>
+        <v>0102_1_1</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!J31</f>
+        <v>0102_1_2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More Gamma-irrad measurements, TempVariation
</commit_message>
<xml_diff>
--- a/SampleInfo.xlsx
+++ b/SampleInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Received Dose" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,13 +19,15 @@
     <sheet name="Gamma_1Gy_141020" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Gamma_All_141021" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Gamma_All_141022" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="TempVariation_141024" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Pre-irrad_2_141024" sheetId="13" state="visible" r:id="rId14"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="337">
   <si>
     <t>Irradiation #</t>
   </si>
@@ -612,10 +614,10 @@
     <t>0102_REF1</t>
   </si>
   <si>
-    <t>0200_REF1</t>
-  </si>
-  <si>
-    <t>0202_REF1</t>
+    <t>0140_REF1</t>
+  </si>
+  <si>
+    <t>0142_REF1</t>
   </si>
   <si>
     <t>1000_REF1</t>
@@ -636,10 +638,10 @@
     <t>0102_REF2</t>
   </si>
   <si>
-    <t>0200_REF2</t>
-  </si>
-  <si>
-    <t>0202_REF2</t>
+    <t>0140_REF2</t>
+  </si>
+  <si>
+    <t>0142_REF2</t>
   </si>
   <si>
     <t>1000_REF2</t>
@@ -1012,6 +1014,30 @@
   </si>
   <si>
     <t>Other options for calibration markers in the vial layout; H-3 source, C-14 source, plastic scintillator.</t>
+  </si>
+  <si>
+    <t>Measurement Number</t>
+  </si>
+  <si>
+    <t>SampleID</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Started ~0 C, warming</t>
+  </si>
+  <si>
+    <t>Room Temperature</t>
+  </si>
+  <si>
+    <t>Started ~50 C, cooling</t>
+  </si>
+  <si>
+    <t>STD_3_H</t>
+  </si>
+  <si>
+    <t>STD_14_C</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1171,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1199,6 +1225,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1719,7 +1749,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2083,6 +2113,1157 @@
         <v>HDPE_0_1</v>
       </c>
       <c r="L8" s="11"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A27:C45"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="C2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="D2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D2</f>
+        <v>0052_1F14</v>
+      </c>
+      <c r="E2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="F2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F2</f>
+        <v>0052_2F14</v>
+      </c>
+      <c r="G2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="H2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H2</f>
+        <v>0052_3F14</v>
+      </c>
+      <c r="I2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="J2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J2</f>
+        <v>0052_4F14</v>
+      </c>
+      <c r="K2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="L2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L2</f>
+        <v>0102_1F25</v>
+      </c>
+      <c r="M2" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B3</f>
+        <v>0102_2F25</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="D3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="E3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E3</f>
+        <v>0102_3F25</v>
+      </c>
+      <c r="F3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="G3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G3</f>
+        <v>0102_4F25</v>
+      </c>
+      <c r="H3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="I3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I3</f>
+        <v>0142_1F33</v>
+      </c>
+      <c r="J3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="K3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K3</f>
+        <v>0142_2F33</v>
+      </c>
+      <c r="L3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+      <c r="M3" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M3</f>
+        <v>0142_3F33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="C4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C4</f>
+        <v>0142_4F33</v>
+      </c>
+      <c r="D4" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="F4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F4</f>
+        <v>1002_1F35</v>
+      </c>
+      <c r="G4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="H4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H4</f>
+        <v>1002_2F35</v>
+      </c>
+      <c r="I4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="J4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J4</f>
+        <v>1002_3F35</v>
+      </c>
+      <c r="K4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="L4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L4</f>
+        <v>1002_4F35</v>
+      </c>
+      <c r="M4" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B5</f>
+        <v>0052_1R14</v>
+      </c>
+      <c r="C5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="D5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D5</f>
+        <v>0052_2R14</v>
+      </c>
+      <c r="E5" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="G5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G5</f>
+        <v>0052_3R14</v>
+      </c>
+      <c r="H5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="I5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I5</f>
+        <v>0052_4R14</v>
+      </c>
+      <c r="J5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="K5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K5</f>
+        <v>0102_1R25</v>
+      </c>
+      <c r="L5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+      <c r="M5" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M5</f>
+        <v>0102_2R25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="C6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C6</f>
+        <v>0102_3R25</v>
+      </c>
+      <c r="D6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="E6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E6</f>
+        <v>0102_4R25</v>
+      </c>
+      <c r="F6" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="H6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H6</f>
+        <v>0142_1R33</v>
+      </c>
+      <c r="I6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="J6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J6</f>
+        <v>0142_2R33</v>
+      </c>
+      <c r="K6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="L6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L6</f>
+        <v>0142_3R33</v>
+      </c>
+      <c r="M6" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B7</f>
+        <v>0142_4R33</v>
+      </c>
+      <c r="C7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="D7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D7</f>
+        <v>1002_1R35</v>
+      </c>
+      <c r="E7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="F7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F7</f>
+        <v>1002_2R35</v>
+      </c>
+      <c r="G7" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="I7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I7</f>
+        <v>1002_3R35</v>
+      </c>
+      <c r="J7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="K7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K7</f>
+        <v>1002_4R35</v>
+      </c>
+      <c r="L7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="C8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C8</f>
+        <v>0052_1F12</v>
+      </c>
+      <c r="D8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="E8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E8</f>
+        <v>0052_2F12</v>
+      </c>
+      <c r="F8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="G8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G8</f>
+        <v>0052_3F12</v>
+      </c>
+      <c r="H8" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="J8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J8</f>
+        <v>0052_4F12</v>
+      </c>
+      <c r="K8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="L8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L8</f>
+        <v>0102_1F21</v>
+      </c>
+      <c r="M8" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B9</f>
+        <v>0102_2F21</v>
+      </c>
+      <c r="C9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="D9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D9</f>
+        <v>0102_3F21</v>
+      </c>
+      <c r="E9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="F9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F9</f>
+        <v>0102_4F21</v>
+      </c>
+      <c r="G9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="H9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H9</f>
+        <v>0142_1F26</v>
+      </c>
+      <c r="I9" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+      <c r="K9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K9</f>
+        <v>0142_2F26</v>
+      </c>
+      <c r="L9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L9</f>
+        <v>0140_3F31</v>
+      </c>
+      <c r="M9" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M9</f>
+        <v>0142_3F26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B10</f>
+        <v>0140_4F31</v>
+      </c>
+      <c r="C10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C10</f>
+        <v>0142_4F26</v>
+      </c>
+      <c r="D10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="E10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E10</f>
+        <v>1002_1F32</v>
+      </c>
+      <c r="F10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="G10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G10</f>
+        <v>1002_2F32</v>
+      </c>
+      <c r="H10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H10</f>
+        <v>1000_3F36</v>
+      </c>
+      <c r="I10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I10</f>
+        <v>1002_3F32</v>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="K10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K10</f>
+        <v>1000_4F36</v>
+      </c>
+      <c r="L10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L10</f>
+        <v>1002_4F32</v>
+      </c>
+      <c r="M10" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B11</f>
+        <v>0052_1R12</v>
+      </c>
+      <c r="C11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="D11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D11</f>
+        <v>0052_2R12</v>
+      </c>
+      <c r="E11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="F11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F11</f>
+        <v>0052_3R12</v>
+      </c>
+      <c r="G11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="H11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H11</f>
+        <v>0052_4R12</v>
+      </c>
+      <c r="I11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="J11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J11</f>
+        <v>0102_1R21</v>
+      </c>
+      <c r="K11" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+      <c r="M11" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M11</f>
+        <v>0102_2R21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="C12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C12</f>
+        <v>0102_3R21</v>
+      </c>
+      <c r="D12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="E12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E12</f>
+        <v>0102_4R21</v>
+      </c>
+      <c r="F12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="G12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G12</f>
+        <v>0142_1R26</v>
+      </c>
+      <c r="H12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="I12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I12</f>
+        <v>0142_2R26</v>
+      </c>
+      <c r="J12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J12</f>
+        <v>0140_3R31</v>
+      </c>
+      <c r="K12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K12</f>
+        <v>0142_3R26</v>
+      </c>
+      <c r="L12" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L12</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M12" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M12</f>
+        <v>0140_4R31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B13</f>
+        <v>0142_4R26</v>
+      </c>
+      <c r="C13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="D13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D13</f>
+        <v>1002_1R32</v>
+      </c>
+      <c r="E13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="F13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F13</f>
+        <v>1002_2R32</v>
+      </c>
+      <c r="G13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G13</f>
+        <v>1000_3R36</v>
+      </c>
+      <c r="H13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H13</f>
+        <v>1002_3R32</v>
+      </c>
+      <c r="I13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I13</f>
+        <v>1000_4R36</v>
+      </c>
+      <c r="J13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J13</f>
+        <v>1002_4R32</v>
+      </c>
+      <c r="K13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="L13" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L13</f>
+        <v>0052_1F17</v>
+      </c>
+      <c r="M13" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C16</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E16</f>
+        <v>0052_2F17</v>
+      </c>
+      <c r="F14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F16</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="G14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G16</f>
+        <v>0052_3F17</v>
+      </c>
+      <c r="H14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H16</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="I14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I16</f>
+        <v>0052_4F17</v>
+      </c>
+      <c r="J14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J16</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K16</f>
+        <v>0100_2F27</v>
+      </c>
+      <c r="L14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L16</f>
+        <v>0100_3F27</v>
+      </c>
+      <c r="M14" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M16</f>
+        <v>0100_4F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="I15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I15</f>
+        <v>0052_1R17</v>
+      </c>
+      <c r="J15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="K15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K15</f>
+        <v>0052_2R17</v>
+      </c>
+      <c r="L15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+      <c r="M15" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M15</f>
+        <v>0052_3R17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C14</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="D16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D14</f>
+        <v>0052_4R17</v>
+      </c>
+      <c r="E16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E14</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="9" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G14</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="H16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H14</f>
+        <v>0100_3R27</v>
+      </c>
+      <c r="I16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I14</f>
+        <v>0100_4R27</v>
+      </c>
+      <c r="J16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J14</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K14</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L14</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="11" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M14</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!C17</f>
+        <v>0052_REF1</v>
+      </c>
+      <c r="D17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!E17</f>
+        <v>0102_REF1</v>
+      </c>
+      <c r="F17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!G17</f>
+        <v>0142_REF1</v>
+      </c>
+      <c r="H17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!I17</f>
+        <v>1002_REF1</v>
+      </c>
+      <c r="J17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!J17</f>
+        <v>0050_REF2</v>
+      </c>
+      <c r="K17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!K17</f>
+        <v>0052_REF2</v>
+      </c>
+      <c r="L17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!L17</f>
+        <v>0100_REF2</v>
+      </c>
+      <c r="M17" s="14" t="str">
+        <f aca="false">'Pre-irrad_1_141014'!M17</f>
+        <v>0102_REF2</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2243,7 +3424,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I42" activeCellId="0" sqref="I42"/>
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3202,7 +4383,7 @@
   </sheetPr>
   <dimension ref="1:73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -6093,11 +7274,11 @@
       </c>
       <c r="F18" s="7" t="str">
         <f aca="false">HolderMatrix!E34</f>
-        <v>0200_REF1</v>
+        <v>0140_REF1</v>
       </c>
       <c r="G18" s="7" t="str">
         <f aca="false">HolderMatrix!F34</f>
-        <v>0202_REF1</v>
+        <v>0142_REF1</v>
       </c>
       <c r="H18" s="7" t="str">
         <f aca="false">HolderMatrix!G34</f>
@@ -8016,11 +9197,11 @@
       </c>
       <c r="F73" s="7" t="str">
         <f aca="false">F18</f>
-        <v>0200_REF1</v>
+        <v>0140_REF1</v>
       </c>
       <c r="G73" s="7" t="str">
         <f aca="false">G18</f>
-        <v>0202_REF1</v>
+        <v>0142_REF1</v>
       </c>
       <c r="H73" s="7" t="str">
         <f aca="false">H18</f>
@@ -8065,8 +9246,8 @@
   </sheetPr>
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H81" activeCellId="0" sqref="H81"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9206,11 +10387,11 @@
       </c>
       <c r="F58" s="7" t="str">
         <f aca="false">HolderMatrix!E34</f>
-        <v>0200_REF1</v>
+        <v>0140_REF1</v>
       </c>
       <c r="G58" s="7" t="str">
         <f aca="false">HolderMatrix!F34</f>
-        <v>0202_REF1</v>
+        <v>0142_REF1</v>
       </c>
       <c r="H58" s="7" t="str">
         <f aca="false">HolderMatrix!G34</f>
@@ -9243,11 +10424,11 @@
       </c>
       <c r="F59" s="7" t="str">
         <f aca="false">HolderMatrix!E35</f>
-        <v>0200_REF2</v>
+        <v>0140_REF2</v>
       </c>
       <c r="G59" s="7" t="str">
         <f aca="false">HolderMatrix!F35</f>
-        <v>0202_REF2</v>
+        <v>0142_REF2</v>
       </c>
       <c r="H59" s="7" t="str">
         <f aca="false">HolderMatrix!G35</f>
@@ -9777,7 +10958,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10642,11 +11823,11 @@
       </c>
       <c r="F17" s="7" t="str">
         <f aca="false">'LS Measurement arrangement'!F18</f>
-        <v>0200_REF1</v>
+        <v>0140_REF1</v>
       </c>
       <c r="G17" s="7" t="str">
         <f aca="false">'LS Measurement arrangement'!G18</f>
-        <v>0202_REF1</v>
+        <v>0142_REF1</v>
       </c>
       <c r="H17" s="7" t="str">
         <f aca="false">'LS Measurement arrangement'!H18</f>

</xml_diff>

<commit_message>
Corrected Meas on 141022, Added 141024 measurements
SampleInfo now has the correct loading info for the 141022 measurement.
</commit_message>
<xml_diff>
--- a/SampleInfo.xlsx
+++ b/SampleInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Received Dose" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="337">
   <si>
     <t>Irradiation #</t>
   </si>
@@ -1746,10 +1746,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2045,74 +2045,49 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B7" s="11" t="str">
-        <f aca="false">'LS Measurement arrangement'!B52</f>
-        <v>PP_1000_1</v>
-      </c>
-      <c r="C7" s="11" t="str">
-        <f aca="false">'LS Measurement arrangement'!C52</f>
-        <v>PP_1000_2</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="9" t="str">
-        <f aca="false">'LS Measurement arrangement'!G52</f>
-        <v>EMPTY</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B8" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!B53</f>
         <v>LS Vit. C</v>
       </c>
-      <c r="C8" s="11" t="str">
+      <c r="C7" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!C53</f>
         <v>15% WbLS Vit. C</v>
       </c>
-      <c r="D8" s="11" t="str">
+      <c r="D7" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!D53</f>
         <v>10% WbLS Vit. C</v>
       </c>
-      <c r="E8" s="11" t="str">
+      <c r="E7" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!E53</f>
         <v>5% WbLS Vit. C</v>
       </c>
-      <c r="F8" s="11" t="str">
+      <c r="F7" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!F53</f>
         <v>LS 10/20/14</v>
       </c>
-      <c r="G8" s="11" t="str">
+      <c r="G7" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!G53</f>
         <v>WbLS-15 10/20/14</v>
       </c>
-      <c r="H8" s="9" t="str">
+      <c r="H7" s="9" t="str">
         <f aca="false">'LS Measurement arrangement'!H53</f>
         <v>EMPTY</v>
       </c>
-      <c r="I8" s="11" t="str">
+      <c r="I7" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!I53</f>
         <v>WbLS-10 10/20/14</v>
       </c>
-      <c r="J8" s="11" t="str">
+      <c r="J7" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!J53</f>
         <v>WbLS-5 10/20/14</v>
       </c>
-      <c r="K8" s="11" t="str">
+      <c r="K7" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!K53</f>
         <v>HDPE_0_1</v>
       </c>
-      <c r="L8" s="11"/>
+      <c r="L7" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2132,7 +2107,7 @@
   </sheetPr>
   <dimension ref="A27:C45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -2369,8 +2344,8 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
New data, photos, loadings, and temp measurements
Pre-irrad_3_141029 loading and photo
Pre-irrad_4/5_141031 loading, photo, data, and temperature measurements.
</commit_message>
<xml_diff>
--- a/SampleInfo.xlsx
+++ b/SampleInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Received Dose" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,6 +21,9 @@
     <sheet name="Gamma_All_141022" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="TempVariation_141024" sheetId="12" state="visible" r:id="rId13"/>
     <sheet name="Pre-irrad_2_141024" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Pre-irrad_3_141029" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Pre-irrad_4_141031" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Pre-irrad_5_141031" sheetId="16" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -1748,8 +1751,8 @@
   </sheetPr>
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2345,7 +2348,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3237,6 +3240,2841 @@
       </c>
       <c r="M17" s="14" t="str">
         <f aca="false">'Pre-irrad_1_141014'!M17</f>
+        <v>0102_REF2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A1</f>
+        <v>Tray ID</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B1</f>
+        <v>Position 1</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C1</f>
+        <v>Position 2</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D1</f>
+        <v>Position 3</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E1</f>
+        <v>Position 4</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F1</f>
+        <v>Position 5</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G1</f>
+        <v>Position 6</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H1</f>
+        <v>Position 7</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I1</f>
+        <v>Position 8</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J1</f>
+        <v>Position 9</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K1</f>
+        <v>Position 10</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L1</f>
+        <v>Position 11</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M1</f>
+        <v>Position 12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A2</f>
+        <v>S1</v>
+      </c>
+      <c r="B2" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B2</f>
+        <v>STD_3_H</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D2</f>
+        <v>0052_1F14</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F2</f>
+        <v>0052_2F14</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H2</f>
+        <v>0052_3F14</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J2</f>
+        <v>0052_4F14</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L2</f>
+        <v>0102_1F25</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A3</f>
+        <v>S2</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B3</f>
+        <v>0102_2F25</v>
+      </c>
+      <c r="C3" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C3</f>
+        <v>STD_14_C</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E3</f>
+        <v>0102_3F25</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G3</f>
+        <v>0102_4F25</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I3</f>
+        <v>0142_1F33</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K3</f>
+        <v>0142_2F33</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M3</f>
+        <v>0142_3F33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A4</f>
+        <v>S3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C4</f>
+        <v>0142_4F33</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F4</f>
+        <v>1002_1F35</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H4</f>
+        <v>1002_2F35</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J4</f>
+        <v>1002_3F35</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L4</f>
+        <v>1002_4F35</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A5</f>
+        <v>S4</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B5</f>
+        <v>0052_1R14</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D5</f>
+        <v>0052_2R14</v>
+      </c>
+      <c r="E5" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G5</f>
+        <v>0052_3R14</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I5</f>
+        <v>0052_4R14</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K5</f>
+        <v>0102_1R25</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M5</f>
+        <v>0102_2R25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A6</f>
+        <v>S5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C6</f>
+        <v>0102_3R25</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E6</f>
+        <v>0102_4R25</v>
+      </c>
+      <c r="F6" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H6</f>
+        <v>0142_1R33</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J6</f>
+        <v>0142_2R33</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L6</f>
+        <v>0142_3R33</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A7</f>
+        <v>S6</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B7</f>
+        <v>0142_4R33</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D7</f>
+        <v>1002_1R35</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F7</f>
+        <v>1002_2R35</v>
+      </c>
+      <c r="G7" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="I7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I7</f>
+        <v>1002_3R35</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="K7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K7</f>
+        <v>1002_4R35</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A8</f>
+        <v>S7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C8</f>
+        <v>0052_1F12</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E8</f>
+        <v>0052_2F12</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G8</f>
+        <v>0052_3F12</v>
+      </c>
+      <c r="H8" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J8</f>
+        <v>0052_4F12</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L8</f>
+        <v>0102_1F21</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A9</f>
+        <v>S8</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B9</f>
+        <v>0102_2F21</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D9</f>
+        <v>0102_3F21</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F9</f>
+        <v>0102_4F21</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H9</f>
+        <v>0142_1F26</v>
+      </c>
+      <c r="I9" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K9</f>
+        <v>0142_2F26</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L9</f>
+        <v>0140_3F31</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M9</f>
+        <v>0142_3F26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A10</f>
+        <v>S9</v>
+      </c>
+      <c r="B10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B10</f>
+        <v>0140_4F31</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C10</f>
+        <v>0142_4F26</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E10</f>
+        <v>1002_1F32</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="G10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G10</f>
+        <v>1002_2F32</v>
+      </c>
+      <c r="H10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H10</f>
+        <v>1000_3F36</v>
+      </c>
+      <c r="I10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I10</f>
+        <v>1002_3F32</v>
+      </c>
+      <c r="J10" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="K10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K10</f>
+        <v>1000_4F36</v>
+      </c>
+      <c r="L10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L10</f>
+        <v>1002_4F32</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A11</f>
+        <v>S10</v>
+      </c>
+      <c r="B11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B11</f>
+        <v>0052_1R12</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="D11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D11</f>
+        <v>0052_2R12</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="F11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F11</f>
+        <v>0052_3R12</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="H11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H11</f>
+        <v>0052_4R12</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="J11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J11</f>
+        <v>0102_1R21</v>
+      </c>
+      <c r="K11" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+      <c r="M11" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M11</f>
+        <v>0102_2R21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A12</f>
+        <v>S11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C12</f>
+        <v>0102_3R21</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E12</f>
+        <v>0102_4R21</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G12</f>
+        <v>0142_1R26</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="I12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I12</f>
+        <v>0142_2R26</v>
+      </c>
+      <c r="J12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J12</f>
+        <v>0140_3R31</v>
+      </c>
+      <c r="K12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K12</f>
+        <v>0142_3R26</v>
+      </c>
+      <c r="L12" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L12</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M12" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M12</f>
+        <v>0140_4R31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A13</f>
+        <v>S12</v>
+      </c>
+      <c r="B13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B13</f>
+        <v>0142_4R26</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D13</f>
+        <v>1002_1R32</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="F13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F13</f>
+        <v>1002_2R32</v>
+      </c>
+      <c r="G13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G13</f>
+        <v>1000_3R36</v>
+      </c>
+      <c r="H13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H13</f>
+        <v>1002_3R32</v>
+      </c>
+      <c r="I13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I13</f>
+        <v>1000_4R36</v>
+      </c>
+      <c r="J13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J13</f>
+        <v>1002_4R32</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="L13" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L13</f>
+        <v>0052_1F17</v>
+      </c>
+      <c r="M13" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A14</f>
+        <v>S13</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C14</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E14</f>
+        <v>0052_2F17</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F14</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="G14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G14</f>
+        <v>0052_3F17</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H14</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="I14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I14</f>
+        <v>0052_4F17</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J14</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K14</f>
+        <v>0100_2F27</v>
+      </c>
+      <c r="L14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L14</f>
+        <v>0100_3F27</v>
+      </c>
+      <c r="M14" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M14</f>
+        <v>0100_4F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A15</f>
+        <v>S14</v>
+      </c>
+      <c r="B15" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="I15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I15</f>
+        <v>0052_1R17</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="K15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K15</f>
+        <v>0052_2R17</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+      <c r="M15" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M15</f>
+        <v>0052_3R17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A16</f>
+        <v>S15</v>
+      </c>
+      <c r="B16" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C16</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="D16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D16</f>
+        <v>0052_4R17</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E16</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="12" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G16</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="H16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H16</f>
+        <v>0100_3R27</v>
+      </c>
+      <c r="I16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I16</f>
+        <v>0100_4R27</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J16</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K16</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L16</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M16</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!A17</f>
+        <v>R1</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!C17</f>
+        <v>0052_REF1</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!E17</f>
+        <v>0102_REF1</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!G17</f>
+        <v>0142_REF1</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!I17</f>
+        <v>1002_REF1</v>
+      </c>
+      <c r="J17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!J17</f>
+        <v>0050_REF2</v>
+      </c>
+      <c r="K17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!K17</f>
+        <v>0052_REF2</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!L17</f>
+        <v>0100_REF2</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f aca="false">'Pre-irrad_2_141024'!M17</f>
+        <v>0102_REF2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A1</f>
+        <v>Tray ID</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B1</f>
+        <v>Position 1</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C1</f>
+        <v>Position 2</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D1</f>
+        <v>Position 3</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E1</f>
+        <v>Position 4</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F1</f>
+        <v>Position 5</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G1</f>
+        <v>Position 6</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H1</f>
+        <v>Position 7</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I1</f>
+        <v>Position 8</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J1</f>
+        <v>Position 9</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K1</f>
+        <v>Position 10</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L1</f>
+        <v>Position 11</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M1</f>
+        <v>Position 12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A2</f>
+        <v>S1</v>
+      </c>
+      <c r="B2" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B2</f>
+        <v>STD_3_H</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D2</f>
+        <v>0052_1F14</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F2</f>
+        <v>0052_2F14</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H2</f>
+        <v>0052_3F14</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J2</f>
+        <v>0052_4F14</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L2</f>
+        <v>0102_1F25</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A3</f>
+        <v>S2</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B3</f>
+        <v>0102_2F25</v>
+      </c>
+      <c r="C3" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C3</f>
+        <v>STD_14_C</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E3</f>
+        <v>0102_3F25</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G3</f>
+        <v>0102_4F25</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I3</f>
+        <v>0142_1F33</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K3</f>
+        <v>0142_2F33</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M3</f>
+        <v>0142_3F33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A4</f>
+        <v>S3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C4</f>
+        <v>0142_4F33</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F4</f>
+        <v>1002_1F35</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H4</f>
+        <v>1002_2F35</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J4</f>
+        <v>1002_3F35</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L4</f>
+        <v>1002_4F35</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A5</f>
+        <v>S4</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B5</f>
+        <v>0052_1R14</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D5</f>
+        <v>0052_2R14</v>
+      </c>
+      <c r="E5" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G5</f>
+        <v>0052_3R14</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I5</f>
+        <v>0052_4R14</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K5</f>
+        <v>0102_1R25</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M5</f>
+        <v>0102_2R25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A6</f>
+        <v>S5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C6</f>
+        <v>0102_3R25</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E6</f>
+        <v>0102_4R25</v>
+      </c>
+      <c r="F6" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H6</f>
+        <v>0142_1R33</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J6</f>
+        <v>0142_2R33</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L6</f>
+        <v>0142_3R33</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A7</f>
+        <v>S6</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B7</f>
+        <v>0142_4R33</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D7</f>
+        <v>1002_1R35</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F7</f>
+        <v>1002_2R35</v>
+      </c>
+      <c r="G7" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="I7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I7</f>
+        <v>1002_3R35</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="K7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K7</f>
+        <v>1002_4R35</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A8</f>
+        <v>S7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C8</f>
+        <v>0052_1F12</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E8</f>
+        <v>0052_2F12</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G8</f>
+        <v>0052_3F12</v>
+      </c>
+      <c r="H8" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J8</f>
+        <v>0052_4F12</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L8</f>
+        <v>0102_1F21</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A9</f>
+        <v>S8</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B9</f>
+        <v>0102_2F21</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D9</f>
+        <v>0102_3F21</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F9</f>
+        <v>0102_4F21</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H9</f>
+        <v>0142_1F26</v>
+      </c>
+      <c r="I9" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K9</f>
+        <v>0142_2F26</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L9</f>
+        <v>0140_3F31</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M9</f>
+        <v>0142_3F26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A10</f>
+        <v>S9</v>
+      </c>
+      <c r="B10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B10</f>
+        <v>0140_4F31</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C10</f>
+        <v>0142_4F26</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E10</f>
+        <v>1002_1F32</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="G10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G10</f>
+        <v>1002_2F32</v>
+      </c>
+      <c r="H10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H10</f>
+        <v>1000_3F36</v>
+      </c>
+      <c r="I10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I10</f>
+        <v>1002_3F32</v>
+      </c>
+      <c r="J10" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="K10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K10</f>
+        <v>1000_4F36</v>
+      </c>
+      <c r="L10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L10</f>
+        <v>1002_4F32</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A11</f>
+        <v>S10</v>
+      </c>
+      <c r="B11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B11</f>
+        <v>0052_1R12</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="D11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D11</f>
+        <v>0052_2R12</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="F11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F11</f>
+        <v>0052_3R12</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="H11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H11</f>
+        <v>0052_4R12</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="J11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J11</f>
+        <v>0102_1R21</v>
+      </c>
+      <c r="K11" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+      <c r="M11" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M11</f>
+        <v>0102_2R21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A12</f>
+        <v>S11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C12</f>
+        <v>0102_3R21</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E12</f>
+        <v>0102_4R21</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G12</f>
+        <v>0142_1R26</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="I12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I12</f>
+        <v>0142_2R26</v>
+      </c>
+      <c r="J12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J12</f>
+        <v>0140_3R31</v>
+      </c>
+      <c r="K12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K12</f>
+        <v>0142_3R26</v>
+      </c>
+      <c r="L12" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L12</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M12" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M12</f>
+        <v>0140_4R31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A13</f>
+        <v>S12</v>
+      </c>
+      <c r="B13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B13</f>
+        <v>0142_4R26</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D13</f>
+        <v>1002_1R32</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="F13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F13</f>
+        <v>1002_2R32</v>
+      </c>
+      <c r="G13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G13</f>
+        <v>1000_3R36</v>
+      </c>
+      <c r="H13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H13</f>
+        <v>1002_3R32</v>
+      </c>
+      <c r="I13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I13</f>
+        <v>1000_4R36</v>
+      </c>
+      <c r="J13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J13</f>
+        <v>1002_4R32</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="L13" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L13</f>
+        <v>0052_1F17</v>
+      </c>
+      <c r="M13" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A14</f>
+        <v>S13</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C14</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E14</f>
+        <v>0052_2F17</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F14</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="G14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G14</f>
+        <v>0052_3F17</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H14</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="I14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I14</f>
+        <v>0052_4F17</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J14</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K14</f>
+        <v>0100_2F27</v>
+      </c>
+      <c r="L14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L14</f>
+        <v>0100_3F27</v>
+      </c>
+      <c r="M14" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M14</f>
+        <v>0100_4F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A15</f>
+        <v>S14</v>
+      </c>
+      <c r="B15" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="I15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I15</f>
+        <v>0052_1R17</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="K15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K15</f>
+        <v>0052_2R17</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+      <c r="M15" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M15</f>
+        <v>0052_3R17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A16</f>
+        <v>S15</v>
+      </c>
+      <c r="B16" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C16</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="D16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D16</f>
+        <v>0052_4R17</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E16</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="12" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G16</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="H16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H16</f>
+        <v>0100_3R27</v>
+      </c>
+      <c r="I16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I16</f>
+        <v>0100_4R27</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J16</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K16</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L16</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M16</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!A17</f>
+        <v>R1</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!C17</f>
+        <v>0052_REF1</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!E17</f>
+        <v>0102_REF1</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!G17</f>
+        <v>0142_REF1</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!I17</f>
+        <v>1002_REF1</v>
+      </c>
+      <c r="J17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!J17</f>
+        <v>0050_REF2</v>
+      </c>
+      <c r="K17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!K17</f>
+        <v>0052_REF2</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!L17</f>
+        <v>0100_REF2</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f aca="false">'Pre-irrad_3_141029'!M17</f>
+        <v>0102_REF2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A1</f>
+        <v>Tray ID</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B1</f>
+        <v>Position 1</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C1</f>
+        <v>Position 2</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D1</f>
+        <v>Position 3</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E1</f>
+        <v>Position 4</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F1</f>
+        <v>Position 5</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G1</f>
+        <v>Position 6</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H1</f>
+        <v>Position 7</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I1</f>
+        <v>Position 8</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J1</f>
+        <v>Position 9</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K1</f>
+        <v>Position 10</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L1</f>
+        <v>Position 11</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M1</f>
+        <v>Position 12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A2</f>
+        <v>S1</v>
+      </c>
+      <c r="B2" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B2</f>
+        <v>STD_3_H</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="D2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D2</f>
+        <v>0052_1F14</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="F2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F2</f>
+        <v>0052_2F14</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="H2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H2</f>
+        <v>0052_3F14</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="J2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J2</f>
+        <v>0052_4F14</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="L2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L2</f>
+        <v>0102_1F25</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A3</f>
+        <v>S2</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B3</f>
+        <v>0102_2F25</v>
+      </c>
+      <c r="C3" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C3</f>
+        <v>STD_14_C</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="E3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E3</f>
+        <v>0102_3F25</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="G3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G3</f>
+        <v>0102_4F25</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="I3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I3</f>
+        <v>0142_1F33</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K3</f>
+        <v>0142_2F33</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+      <c r="M3" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M3</f>
+        <v>0142_3F33</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A4</f>
+        <v>S3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C4</f>
+        <v>0142_4F33</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="F4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F4</f>
+        <v>1002_1F35</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="H4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H4</f>
+        <v>1002_2F35</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="J4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J4</f>
+        <v>1002_3F35</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="L4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L4</f>
+        <v>1002_4F35</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A5</f>
+        <v>S4</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B5</f>
+        <v>0052_1R14</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="D5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D5</f>
+        <v>0052_2R14</v>
+      </c>
+      <c r="E5" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="G5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G5</f>
+        <v>0052_3R14</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="I5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I5</f>
+        <v>0052_4R14</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K5</f>
+        <v>0102_1R25</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+      <c r="M5" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M5</f>
+        <v>0102_2R25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A6</f>
+        <v>S5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C6</f>
+        <v>0102_3R25</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="E6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E6</f>
+        <v>0102_4R25</v>
+      </c>
+      <c r="F6" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="H6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H6</f>
+        <v>0142_1R33</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="J6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J6</f>
+        <v>0142_2R33</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="L6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L6</f>
+        <v>0142_3R33</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A7</f>
+        <v>S6</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B7</f>
+        <v>0142_4R33</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="D7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D7</f>
+        <v>1002_1R35</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="F7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F7</f>
+        <v>1002_2R35</v>
+      </c>
+      <c r="G7" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="I7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I7</f>
+        <v>1002_3R35</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="K7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K7</f>
+        <v>1002_4R35</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A8</f>
+        <v>S7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C8</f>
+        <v>0052_1F12</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="E8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E8</f>
+        <v>0052_2F12</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="G8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G8</f>
+        <v>0052_3F12</v>
+      </c>
+      <c r="H8" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="J8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J8</f>
+        <v>0052_4F12</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="L8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L8</f>
+        <v>0102_1F21</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A9</f>
+        <v>S8</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B9</f>
+        <v>0102_2F21</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="D9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D9</f>
+        <v>0102_3F21</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="F9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F9</f>
+        <v>0102_4F21</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="H9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H9</f>
+        <v>0142_1F26</v>
+      </c>
+      <c r="I9" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+      <c r="K9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K9</f>
+        <v>0142_2F26</v>
+      </c>
+      <c r="L9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L9</f>
+        <v>0140_3F31</v>
+      </c>
+      <c r="M9" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M9</f>
+        <v>0142_3F26</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A10</f>
+        <v>S9</v>
+      </c>
+      <c r="B10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B10</f>
+        <v>0140_4F31</v>
+      </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C10</f>
+        <v>0142_4F26</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="E10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E10</f>
+        <v>1002_1F32</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="G10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G10</f>
+        <v>1002_2F32</v>
+      </c>
+      <c r="H10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H10</f>
+        <v>1000_3F36</v>
+      </c>
+      <c r="I10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I10</f>
+        <v>1002_3F32</v>
+      </c>
+      <c r="J10" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="K10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K10</f>
+        <v>1000_4F36</v>
+      </c>
+      <c r="L10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L10</f>
+        <v>1002_4F32</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A11</f>
+        <v>S10</v>
+      </c>
+      <c r="B11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B11</f>
+        <v>0052_1R12</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="D11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D11</f>
+        <v>0052_2R12</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="F11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F11</f>
+        <v>0052_3R12</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="H11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H11</f>
+        <v>0052_4R12</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="J11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J11</f>
+        <v>0102_1R21</v>
+      </c>
+      <c r="K11" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+      <c r="M11" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M11</f>
+        <v>0102_2R21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A12</f>
+        <v>S11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C12</f>
+        <v>0102_3R21</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="E12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E12</f>
+        <v>0102_4R21</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="G12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G12</f>
+        <v>0142_1R26</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="I12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I12</f>
+        <v>0142_2R26</v>
+      </c>
+      <c r="J12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J12</f>
+        <v>0140_3R31</v>
+      </c>
+      <c r="K12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K12</f>
+        <v>0142_3R26</v>
+      </c>
+      <c r="L12" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L12</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M12" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M12</f>
+        <v>0140_4R31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A13</f>
+        <v>S12</v>
+      </c>
+      <c r="B13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B13</f>
+        <v>0142_4R26</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="D13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D13</f>
+        <v>1002_1R32</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="F13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F13</f>
+        <v>1002_2R32</v>
+      </c>
+      <c r="G13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G13</f>
+        <v>1000_3R36</v>
+      </c>
+      <c r="H13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H13</f>
+        <v>1002_3R32</v>
+      </c>
+      <c r="I13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I13</f>
+        <v>1000_4R36</v>
+      </c>
+      <c r="J13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J13</f>
+        <v>1002_4R32</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="L13" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L13</f>
+        <v>0052_1F17</v>
+      </c>
+      <c r="M13" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A14</f>
+        <v>S13</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C14</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E14</f>
+        <v>0052_2F17</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F14</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="G14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G14</f>
+        <v>0052_3F17</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H14</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="I14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I14</f>
+        <v>0052_4F17</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J14</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K14</f>
+        <v>0100_2F27</v>
+      </c>
+      <c r="L14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L14</f>
+        <v>0100_3F27</v>
+      </c>
+      <c r="M14" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M14</f>
+        <v>0100_4F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A15</f>
+        <v>S14</v>
+      </c>
+      <c r="B15" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="I15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I15</f>
+        <v>0052_1R17</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="K15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K15</f>
+        <v>0052_2R17</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+      <c r="M15" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M15</f>
+        <v>0052_3R17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A16</f>
+        <v>S15</v>
+      </c>
+      <c r="B16" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C16</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="D16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D16</f>
+        <v>0052_4R17</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E16</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="12" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G16</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="H16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H16</f>
+        <v>0100_3R27</v>
+      </c>
+      <c r="I16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I16</f>
+        <v>0100_4R27</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J16</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K16</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L16</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M16</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!A17</f>
+        <v>R1</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!C17</f>
+        <v>0052_REF1</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!E17</f>
+        <v>0102_REF1</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!G17</f>
+        <v>0142_REF1</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!I17</f>
+        <v>1002_REF1</v>
+      </c>
+      <c r="J17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!J17</f>
+        <v>0050_REF2</v>
+      </c>
+      <c r="K17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!K17</f>
+        <v>0052_REF2</v>
+      </c>
+      <c r="L17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!L17</f>
+        <v>0100_REF2</v>
+      </c>
+      <c r="M17" s="7" t="str">
+        <f aca="false">'Pre-irrad_4_141031'!M17</f>
         <v>0102_REF2</v>
       </c>
     </row>
@@ -4358,8 +7196,8 @@
   </sheetPr>
   <dimension ref="1:73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Modified loading of Gamma_All_* runs
The 400 Gy 5% and 5%+AA vials were swapped
</commit_message>
<xml_diff>
--- a/SampleInfo.xlsx
+++ b/SampleInfo.xlsx
@@ -1381,7 +1381,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1470,30 +1470,30 @@
         <f aca="false">'LS Measurement arrangement'!J36</f>
         <v>0052_100_2</v>
       </c>
-      <c r="K2" s="0" t="str">
-        <f aca="false">'LS Measurement arrangement'!K36</f>
-        <v>0050_400_1</v>
+      <c r="K2" s="11" t="str">
+        <f aca="false">'LS Measurement arrangement'!B37</f>
+        <v>0052_400_1</v>
       </c>
       <c r="L2" s="0" t="str">
-        <f aca="false">'LS Measurement arrangement'!L36</f>
-        <v>0050_400_2</v>
+        <f aca="false">'LS Measurement arrangement'!D37</f>
+        <v>0052_400_2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="11" t="str">
-        <f aca="false">'LS Measurement arrangement'!B37</f>
-        <v>0052_400_1</v>
+      <c r="B3" s="0" t="str">
+        <f aca="false">'LS Measurement arrangement'!K36</f>
+        <v>0050_400_1</v>
       </c>
       <c r="C3" s="12" t="str">
         <f aca="false">'LS Measurement arrangement'!C37</f>
         <v>EMPTY</v>
       </c>
       <c r="D3" s="0" t="str">
-        <f aca="false">'LS Measurement arrangement'!D37</f>
-        <v>0052_400_2</v>
+        <f aca="false">'LS Measurement arrangement'!L36</f>
+        <v>0050_400_2</v>
       </c>
       <c r="E3" s="0" t="str">
         <f aca="false">'LS Measurement arrangement'!E37</f>
@@ -1752,7 +1752,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1842,12 +1842,12 @@
         <v>0052_100_2</v>
       </c>
       <c r="K2" s="11" t="str">
-        <f aca="false">'LS Measurement arrangement'!K47</f>
-        <v>0050_400_1</v>
+        <f aca="false">'LS Measurement arrangement'!B48</f>
+        <v>0052_400_1</v>
       </c>
       <c r="L2" s="11" t="str">
-        <f aca="false">'LS Measurement arrangement'!L47</f>
-        <v>0050_400_2</v>
+        <f aca="false">'LS Measurement arrangement'!D48</f>
+        <v>0052_400_2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,16 +1855,16 @@
         <v>226</v>
       </c>
       <c r="B3" s="11" t="str">
-        <f aca="false">'LS Measurement arrangement'!B48</f>
-        <v>0052_400_1</v>
+        <f aca="false">'LS Measurement arrangement'!K47</f>
+        <v>0050_400_1</v>
       </c>
       <c r="C3" s="9" t="str">
         <f aca="false">'LS Measurement arrangement'!C48</f>
         <v>EMPTY</v>
       </c>
       <c r="D3" s="11" t="str">
-        <f aca="false">'LS Measurement arrangement'!D48</f>
-        <v>0052_400_2</v>
+        <f aca="false">'LS Measurement arrangement'!L47</f>
+        <v>0050_400_2</v>
       </c>
       <c r="E3" s="11" t="str">
         <f aca="false">'LS Measurement arrangement'!E48</f>
@@ -5152,7 +5152,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -7196,8 +7196,8 @@
   </sheetPr>
   <dimension ref="1:73"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Updated loading diagrams for runs 9--11
</commit_message>
<xml_diff>
--- a/SampleInfo.xlsx
+++ b/SampleInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Received Dose" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,13 +28,16 @@
     <sheet name="Pre-irrad_6_141105" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="Pre-irrad_7_141106" sheetId="19" state="visible" r:id="rId20"/>
     <sheet name="Pre-irrad_8_141107" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="Pre-irrad_9_141110" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Pre-irrad_10_141113" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="Pre-irrad_11_141114" sheetId="23" state="visible" r:id="rId24"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="338">
   <si>
     <t>Irradiation #</t>
   </si>
@@ -6216,7 +6219,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8245,8 +8248,8 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -8810,6 +8813,1785 @@
       </c>
       <c r="H17" s="7" t="str">
         <f aca="false">'Pre-irrad_7_141106'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A1</f>
+        <v>Tray ID</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B1</f>
+        <v>Position 1</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C1</f>
+        <v>Position 2</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D1</f>
+        <v>Position 3</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E1</f>
+        <v>Position 4</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F1</f>
+        <v>Position 5</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G1</f>
+        <v>Position 6</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H1</f>
+        <v>Position 7</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!I1</f>
+        <v>Position 8</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J1</f>
+        <v>Position 9</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K1</f>
+        <v>Position 10</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!L1</f>
+        <v>Position 11</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M1</f>
+        <v>Position 12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A2</f>
+        <v>S1</v>
+      </c>
+      <c r="B2" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B2</f>
+        <v>STD_3_H</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A3</f>
+        <v>S2</v>
+      </c>
+      <c r="C3" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C3</f>
+        <v>STD_14_C</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A4</f>
+        <v>S3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="D4" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A5</f>
+        <v>S4</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A6</f>
+        <v>S5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="F6" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A7</f>
+        <v>S6</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="G7" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A8</f>
+        <v>S7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="H8" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A9</f>
+        <v>S8</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="I9" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A10</f>
+        <v>S9</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="J10" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A11</f>
+        <v>S10</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="K11" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A12</f>
+        <v>S11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="L12" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!L12</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A13</f>
+        <v>S12</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="M13" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A14</f>
+        <v>S13</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C14</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F14</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H14</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J14</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K14</f>
+        <v>0100_2F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A15</f>
+        <v>S14</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A16</f>
+        <v>S15</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!C16</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!E16</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="13" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!G16</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!J16</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!K16</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!L16</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!M16</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!A17</f>
+        <v>R1</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'Pre-irrad_8_141107'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A1</f>
+        <v>Tray ID</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B1</f>
+        <v>Position 1</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C1</f>
+        <v>Position 2</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D1</f>
+        <v>Position 3</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E1</f>
+        <v>Position 4</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F1</f>
+        <v>Position 5</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G1</f>
+        <v>Position 6</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H1</f>
+        <v>Position 7</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!I1</f>
+        <v>Position 8</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J1</f>
+        <v>Position 9</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K1</f>
+        <v>Position 10</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!L1</f>
+        <v>Position 11</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M1</f>
+        <v>Position 12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A2</f>
+        <v>S1</v>
+      </c>
+      <c r="B2" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B2</f>
+        <v>STD_3_H</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A3</f>
+        <v>S2</v>
+      </c>
+      <c r="C3" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C3</f>
+        <v>STD_14_C</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A4</f>
+        <v>S3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="D4" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A5</f>
+        <v>S4</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A6</f>
+        <v>S5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="F6" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A7</f>
+        <v>S6</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="G7" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A8</f>
+        <v>S7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="H8" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A9</f>
+        <v>S8</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="I9" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A10</f>
+        <v>S9</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="J10" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A11</f>
+        <v>S10</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="K11" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A12</f>
+        <v>S11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="L12" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!L12</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A13</f>
+        <v>S12</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="M13" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A14</f>
+        <v>S13</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C14</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F14</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H14</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J14</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K14</f>
+        <v>0100_2F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A15</f>
+        <v>S14</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A16</f>
+        <v>S15</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!C16</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!E16</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="13" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!G16</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!J16</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!K16</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!L16</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!M16</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!A17</f>
+        <v>R1</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'Pre-irrad_9_141110'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A1</f>
+        <v>Tray ID</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B1</f>
+        <v>Position 1</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C1</f>
+        <v>Position 2</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D1</f>
+        <v>Position 3</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E1</f>
+        <v>Position 4</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F1</f>
+        <v>Position 5</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G1</f>
+        <v>Position 6</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H1</f>
+        <v>Position 7</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!I1</f>
+        <v>Position 8</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J1</f>
+        <v>Position 9</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K1</f>
+        <v>Position 10</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!L1</f>
+        <v>Position 11</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M1</f>
+        <v>Position 12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A2</f>
+        <v>S1</v>
+      </c>
+      <c r="B2" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B2</f>
+        <v>STD_3_H</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A3</f>
+        <v>S2</v>
+      </c>
+      <c r="C3" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C3</f>
+        <v>STD_14_C</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A4</f>
+        <v>S3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="D4" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A5</f>
+        <v>S4</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A6</f>
+        <v>S5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="F6" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A7</f>
+        <v>S6</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="G7" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A8</f>
+        <v>S7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="H8" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A9</f>
+        <v>S8</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="I9" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A10</f>
+        <v>S9</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="J10" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A11</f>
+        <v>S10</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="K11" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A12</f>
+        <v>S11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="L12" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!L12</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A13</f>
+        <v>S12</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="M13" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A14</f>
+        <v>S13</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C14</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F14</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H14</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J14</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K14</f>
+        <v>0100_2F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A15</f>
+        <v>S14</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A16</f>
+        <v>S15</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!C16</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!E16</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="13" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!G16</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!J16</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!K16</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!L16</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!M16</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!A17</f>
+        <v>R1</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'Pre-irrad_10_141113'!H17</f>
         <v>1000_REF1</v>
       </c>
       <c r="I17" s="7" t="s">

</xml_diff>

<commit_message>
Added post-irrad runs 12 and 13, loadings, photos
</commit_message>
<xml_diff>
--- a/SampleInfo.xlsx
+++ b/SampleInfo.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="22"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Received Dose" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,13 +31,15 @@
     <sheet name="Pre-irrad_9_141110" sheetId="21" state="visible" r:id="rId22"/>
     <sheet name="Pre-irrad_10_141113" sheetId="22" state="visible" r:id="rId23"/>
     <sheet name="Pre-irrad_11_141114" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="Post-irrad_12_141117" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="Post-irrad_13_141118" sheetId="25" state="visible" r:id="rId26"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="338">
   <si>
     <t>Irradiation #</t>
   </si>
@@ -10027,7 +10029,7 @@
   </sheetPr>
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -10592,6 +10594,1192 @@
       </c>
       <c r="H17" s="7" t="str">
         <f aca="false">'Pre-irrad_10_141113'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A1</f>
+        <v>Tray ID</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B1</f>
+        <v>Position 1</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C1</f>
+        <v>Position 2</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D1</f>
+        <v>Position 3</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E1</f>
+        <v>Position 4</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F1</f>
+        <v>Position 5</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G1</f>
+        <v>Position 6</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H1</f>
+        <v>Position 7</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!I1</f>
+        <v>Position 8</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J1</f>
+        <v>Position 9</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K1</f>
+        <v>Position 10</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!L1</f>
+        <v>Position 11</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M1</f>
+        <v>Position 12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A2</f>
+        <v>S1</v>
+      </c>
+      <c r="B2" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B2</f>
+        <v>STD_3_H</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A3</f>
+        <v>S2</v>
+      </c>
+      <c r="C3" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C3</f>
+        <v>STD_14_C</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A4</f>
+        <v>S3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="D4" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A5</f>
+        <v>S4</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A6</f>
+        <v>S5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="F6" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A7</f>
+        <v>S6</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="G7" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A8</f>
+        <v>S7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="H8" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A9</f>
+        <v>S8</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="I9" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A10</f>
+        <v>S9</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="J10" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A11</f>
+        <v>S10</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="K11" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A12</f>
+        <v>S11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="L12" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!L12</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A13</f>
+        <v>S12</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="M13" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A14</f>
+        <v>S13</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C14</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F14</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H14</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J14</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K14</f>
+        <v>0100_2F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A15</f>
+        <v>S14</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A16</f>
+        <v>S15</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!C16</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!E16</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="13" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!G16</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!J16</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!K16</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!L16</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!M16</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!A17</f>
+        <v>R1</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'Pre-irrad_11_141114'!H17</f>
+        <v>1000_REF1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M17"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A1</f>
+        <v>Tray ID</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B1</f>
+        <v>Position 1</v>
+      </c>
+      <c r="C1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C1</f>
+        <v>Position 2</v>
+      </c>
+      <c r="D1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D1</f>
+        <v>Position 3</v>
+      </c>
+      <c r="E1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E1</f>
+        <v>Position 4</v>
+      </c>
+      <c r="F1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F1</f>
+        <v>Position 5</v>
+      </c>
+      <c r="G1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G1</f>
+        <v>Position 6</v>
+      </c>
+      <c r="H1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H1</f>
+        <v>Position 7</v>
+      </c>
+      <c r="I1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!I1</f>
+        <v>Position 8</v>
+      </c>
+      <c r="J1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J1</f>
+        <v>Position 9</v>
+      </c>
+      <c r="K1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K1</f>
+        <v>Position 10</v>
+      </c>
+      <c r="L1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!L1</f>
+        <v>Position 11</v>
+      </c>
+      <c r="M1" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M1</f>
+        <v>Position 12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A2</f>
+        <v>S1</v>
+      </c>
+      <c r="B2" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B2</f>
+        <v>STD_3_H</v>
+      </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C2</f>
+        <v>0050_1F13</v>
+      </c>
+      <c r="E2" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E2</f>
+        <v>0050_2F13</v>
+      </c>
+      <c r="G2" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G2</f>
+        <v>0050_3F13</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!I2</f>
+        <v>0050_4F13</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K2</f>
+        <v>0100_1F15</v>
+      </c>
+      <c r="M2" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M2</f>
+        <v>0100_2F15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A3</f>
+        <v>S2</v>
+      </c>
+      <c r="C3" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C3</f>
+        <v>STD_14_C</v>
+      </c>
+      <c r="D3" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D3</f>
+        <v>0100_3F15</v>
+      </c>
+      <c r="F3" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F3</f>
+        <v>0100_4F15</v>
+      </c>
+      <c r="H3" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H3</f>
+        <v>0140_1F23</v>
+      </c>
+      <c r="J3" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J3</f>
+        <v>0140_2F23</v>
+      </c>
+      <c r="L3" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!L3</f>
+        <v>0140_3F23</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A4</f>
+        <v>S3</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B4</f>
+        <v>0140_4F23</v>
+      </c>
+      <c r="D4" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D4</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="E4" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E4</f>
+        <v>1000_1F34</v>
+      </c>
+      <c r="G4" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G4</f>
+        <v>1000_2F34</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!I4</f>
+        <v>1000_3F34</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K4</f>
+        <v>1000_4F34</v>
+      </c>
+      <c r="M4" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M4</f>
+        <v>0050_1R13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A5</f>
+        <v>S4</v>
+      </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C5</f>
+        <v>0050_2R13</v>
+      </c>
+      <c r="E5" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E5</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F5" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F5</f>
+        <v>0050_3R13</v>
+      </c>
+      <c r="H5" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H5</f>
+        <v>0050_4R13</v>
+      </c>
+      <c r="J5" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J5</f>
+        <v>0100_1R15</v>
+      </c>
+      <c r="L5" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!L5</f>
+        <v>0100_2R15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A6</f>
+        <v>S5</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B6</f>
+        <v>0100_3R15</v>
+      </c>
+      <c r="D6" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D6</f>
+        <v>0100_4R15</v>
+      </c>
+      <c r="F6" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F6</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G6" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G6</f>
+        <v>0140_1R23</v>
+      </c>
+      <c r="I6" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!I6</f>
+        <v>0140_2R23</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K6</f>
+        <v>0140_3R23</v>
+      </c>
+      <c r="M6" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M6</f>
+        <v>0140_4R23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A7</f>
+        <v>S6</v>
+      </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C7</f>
+        <v>1000_1R34</v>
+      </c>
+      <c r="E7" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E7</f>
+        <v>1000_2R34</v>
+      </c>
+      <c r="G7" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G7</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="H7" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H7</f>
+        <v>1000_3R34</v>
+      </c>
+      <c r="J7" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J7</f>
+        <v>1000_4R34</v>
+      </c>
+      <c r="L7" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!L7</f>
+        <v>0050_FPMT</v>
+      </c>
+      <c r="M7" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M7</f>
+        <v>0050_RPMT</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A8</f>
+        <v>S7</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B8</f>
+        <v>0050_1F11</v>
+      </c>
+      <c r="D8" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D8</f>
+        <v>0050_2F11</v>
+      </c>
+      <c r="F8" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F8</f>
+        <v>0050_3F11</v>
+      </c>
+      <c r="H8" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H8</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="I8" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!I8</f>
+        <v>0050_4F11</v>
+      </c>
+      <c r="K8" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K8</f>
+        <v>0100_1F22</v>
+      </c>
+      <c r="M8" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M8</f>
+        <v>0100_2F22</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A9</f>
+        <v>S8</v>
+      </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C9</f>
+        <v>0100_3F22</v>
+      </c>
+      <c r="E9" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E9</f>
+        <v>0100_4F22</v>
+      </c>
+      <c r="G9" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G9</f>
+        <v>0140_1F31</v>
+      </c>
+      <c r="I9" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!I9</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="J9" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J9</f>
+        <v>0140_2F31</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A10</f>
+        <v>S9</v>
+      </c>
+      <c r="D10" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D10</f>
+        <v>1000_1F36</v>
+      </c>
+      <c r="F10" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F10</f>
+        <v>1000_2F36</v>
+      </c>
+      <c r="J10" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J10</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="M10" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M10</f>
+        <v>0050_1R11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A11</f>
+        <v>S10</v>
+      </c>
+      <c r="C11" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C11</f>
+        <v>0050_2R11</v>
+      </c>
+      <c r="E11" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E11</f>
+        <v>0050_3R11</v>
+      </c>
+      <c r="G11" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G11</f>
+        <v>0050_4R11</v>
+      </c>
+      <c r="I11" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!I11</f>
+        <v>0100_1R22</v>
+      </c>
+      <c r="K11" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K11</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="L11" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!L11</f>
+        <v>0100_2R22</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A12</f>
+        <v>S11</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B12</f>
+        <v>0100_3R22</v>
+      </c>
+      <c r="D12" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D12</f>
+        <v>0100_4R22</v>
+      </c>
+      <c r="F12" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F12</f>
+        <v>0140_1R31</v>
+      </c>
+      <c r="H12" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H12</f>
+        <v>0140_2R31</v>
+      </c>
+      <c r="L12" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!L12</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A13</f>
+        <v>S12</v>
+      </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C13</f>
+        <v>1000_1R36</v>
+      </c>
+      <c r="E13" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E13</f>
+        <v>1000_2R36</v>
+      </c>
+      <c r="K13" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K13</f>
+        <v>0050_1F16</v>
+      </c>
+      <c r="M13" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M13</f>
+        <v>EMPTY</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A14</f>
+        <v>S13</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C14</f>
+        <v>0050_2F16</v>
+      </c>
+      <c r="D14" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D14</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F14" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F14</f>
+        <v>0050_3F16</v>
+      </c>
+      <c r="H14" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H14</f>
+        <v>0050_4F16</v>
+      </c>
+      <c r="J14" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J14</f>
+        <v>0100_1F27</v>
+      </c>
+      <c r="K14" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K14</f>
+        <v>0100_2F27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A15</f>
+        <v>S14</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C15</f>
+        <v>1000_1F37</v>
+      </c>
+      <c r="D15" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D15</f>
+        <v>1000_2F37</v>
+      </c>
+      <c r="E15" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E15</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="F15" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F15</f>
+        <v>1000_3F37</v>
+      </c>
+      <c r="G15" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G15</f>
+        <v>1000_4F37</v>
+      </c>
+      <c r="H15" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H15</f>
+        <v>0050_1R16</v>
+      </c>
+      <c r="J15" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J15</f>
+        <v>0050_2R16</v>
+      </c>
+      <c r="L15" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!L15</f>
+        <v>0050_3R16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A16</f>
+        <v>S15</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!C16</f>
+        <v>0050_4R16</v>
+      </c>
+      <c r="E16" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!E16</f>
+        <v>0100_1R27</v>
+      </c>
+      <c r="F16" s="13" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F16</f>
+        <v>EMPTY</v>
+      </c>
+      <c r="G16" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!G16</f>
+        <v>0100_2R27</v>
+      </c>
+      <c r="J16" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!J16</f>
+        <v>1000_1R37</v>
+      </c>
+      <c r="K16" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!K16</f>
+        <v>1000_2R37</v>
+      </c>
+      <c r="L16" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!L16</f>
+        <v>1000_3R37</v>
+      </c>
+      <c r="M16" s="0" t="str">
+        <f aca="false">'Post-irrad_12_141117'!M16</f>
+        <v>1000_4R37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="str">
+        <f aca="false">'Post-irrad_12_141117'!A17</f>
+        <v>R1</v>
+      </c>
+      <c r="B17" s="7" t="str">
+        <f aca="false">'Post-irrad_12_141117'!B17</f>
+        <v>0050_REF1</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f aca="false">'Post-irrad_12_141117'!D17</f>
+        <v>0100_REF1</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="F17" s="7" t="str">
+        <f aca="false">'Post-irrad_12_141117'!F17</f>
+        <v>0140_REF1</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H17" s="7" t="str">
+        <f aca="false">'Post-irrad_12_141117'!H17</f>
         <v>1000_REF1</v>
       </c>
       <c r="I17" s="7" t="s">
@@ -11581,7 +12769,7 @@
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>